<commit_message>
add test report + UAT test
</commit_message>
<xml_diff>
--- a/doc/Testcase.xlsx
+++ b/doc/Testcase.xlsx
@@ -5,19 +5,22 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hadez\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Year 3 term 2\Software Engineering\Software_Engineer_PaiNamNae\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6C8FFE2-DD9B-43A9-AA9D-36D86266A0CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8AE530C-8A4F-478F-BB2C-B0BDD67D73BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Scenario Summary" sheetId="1" r:id="rId1"/>
     <sheet name="Defect Summary" sheetId="4" r:id="rId2"/>
     <sheet name="TS001" sheetId="7" r:id="rId3"/>
-    <sheet name="Test Case Design &amp; Test Results" sheetId="3" r:id="rId4"/>
-    <sheet name="Test Summary Report" sheetId="5" r:id="rId5"/>
+    <sheet name="TS002" sheetId="9" r:id="rId4"/>
+    <sheet name="TS003" sheetId="10" r:id="rId5"/>
+    <sheet name="TS004" sheetId="11" r:id="rId6"/>
+    <sheet name="Test Case Design &amp; Test Results" sheetId="3" r:id="rId7"/>
+    <sheet name="Test Summary Report" sheetId="5" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="189">
   <si>
     <t>Scenario ID</t>
   </si>
@@ -367,13 +370,254 @@
     <t>การลบ Account</t>
   </si>
   <si>
-    <t>Log เก็บข้อมูลสำหรับ Admin</t>
-  </si>
-  <si>
     <t>PaiNamNae</t>
   </si>
   <si>
     <t>Testcase No.</t>
+  </si>
+  <si>
+    <t>Step</t>
+  </si>
+  <si>
+    <t>ฟังก์ชันการลบ</t>
+  </si>
+  <si>
+    <t>ฟังก์ชันการส่ง Email</t>
+  </si>
+  <si>
+    <t>นายตะวัน อุตมาน</t>
+  </si>
+  <si>
+    <t>TS002</t>
+  </si>
+  <si>
+    <t>TS003</t>
+  </si>
+  <si>
+    <t>TS004</t>
+  </si>
+  <si>
+    <t>T01</t>
+  </si>
+  <si>
+    <t>สร้าง Table deleteRequest</t>
+  </si>
+  <si>
+    <t>return สถานะ "PENDING"</t>
+  </si>
+  <si>
+    <t>T02</t>
+  </si>
+  <si>
+    <t>T03</t>
+  </si>
+  <si>
+    <t>T04</t>
+  </si>
+  <si>
+    <t>T05</t>
+  </si>
+  <si>
+    <t>T06</t>
+  </si>
+  <si>
+    <t>T07</t>
+  </si>
+  <si>
+    <t>get dataRequest ของ user</t>
+  </si>
+  <si>
+    <t>user-1',        true,
+false,
+false,
+false,
+true</t>
+  </si>
+  <si>
+    <t>user-1</t>
+  </si>
+  <si>
+    <t>return ตาราง deleteRequest โดยที่ userID='user-1'</t>
+  </si>
+  <si>
+    <t>get dataRequest ของ user เมื่อไม่เจอ</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>return Delete request not found</t>
+  </si>
+  <si>
+    <t>อัพเดตคอลัมน์ isDeleted ในตาราง user</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1. Mock ข้อมูลสำหรับ test ใน database   2. เรียกใช้ฟังก์ชัน deleteRequest โดยที่มีข้อมูล userID = "user-1"                         3. ตรวจสอบว่าฟังก์ชันถูกเรียกใช้จริง</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1. Mock ข้อมูลสำหรับ test ใน database   2. เรียกใช้ฟังก์ชัน getDeleteRequest โดยที่มีข้อมูล userID = "null"                        3. ตรวจสอบว่าฟังก์ชันคืนค่าถูก</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1. Mock ข้อมูลสำหรับ test ใน database   2. เรียกใช้ฟังก์ชัน getDeleteRequest โดยที่มีข้อมูล userID = "user-1"                     3. ตรวจสอบว่าฟังก์ชันคืนค่าถูก</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1. Mock ข้อมูลสำหรับ test ใน database   2. เรียกใช้ฟังก์ชัน markDeleteUserData    3. ตรวจสอบว่าค่าในตารางมีการเปลี่ยนแปลง</t>
+  </si>
+  <si>
+    <t>'user-1', deleteRequest</t>
+  </si>
+  <si>
+    <t>ค่า isDeleted = True</t>
+  </si>
+  <si>
+    <t>อัพเดตคอลัมน์ isDeleted ในตาราง vechicle</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1. Mock ข้อมูลสำหรับ test ใน database   2. เรียกใช้ฟังก์ชัน markDeleteVechicles    3. ตรวจสอบว่าค่าในตารางมีการเปลี่ยนแปลง</t>
+  </si>
+  <si>
+    <t>อัพเดตคอลัมน์ isCanceled ในตาราง route</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1. Mock ข้อมูลสำหรับ test ใน database   2. เรียกใช้ฟังก์ชัน markDeleteRoutes       3. ตรวจสอบว่าค่าในตารางมีการเปลี่ยนแปลง</t>
+  </si>
+  <si>
+    <t>ค่า isCanceled = True</t>
+  </si>
+  <si>
+    <t>อัพเดตคอลัมน์ isDeleted ในตาราง booking</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1. Mock ข้อมูลสำหรับ test ใน database   2. เรียกใช้ฟังก์ชัน markDeleteBookings    3. ตรวจสอบว่าค่าในตารางมีการเปลี่ยนแปลง</t>
+  </si>
+  <si>
+    <t>userId</t>
+  </si>
+  <si>
+    <t>ข้อมูลใน row userID</t>
+  </si>
+  <si>
+    <t>userId: 'user-1'</t>
+  </si>
+  <si>
+    <t>deleteRequest</t>
+  </si>
+  <si>
+    <t>สถานะการถูกลบของตารางต่างๆ</t>
+  </si>
+  <si>
+    <t>deleteRequest = { deleteAccount: true }</t>
+  </si>
+  <si>
+    <t>ทดสอบฟังก์ชันการลบใน services</t>
+  </si>
+  <si>
+    <t>ทดสอบการส่งอีเมล</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1. Mock ข้อมูลสำหรับ test ใน database   2. สร้างอีเมลสำหรับทดสอบ                      3. เรียกใช้ฟังก์ชัน                                   4. ตรวจสอบว่าฟังก์ชันคืนค่าถูก</t>
+  </si>
+  <si>
+    <t>to: 'test@example.com',
+subject: 'Test Subject',
+text: 'Hello world',
+attachments: [],</t>
+  </si>
+  <si>
+    <t>ปลายทางได้รับอีเมลของทีม painamnae</t>
+  </si>
+  <si>
+    <t>ได้รับ Error เมื่อส่งอีเมลไม่ได้</t>
+  </si>
+  <si>
+    <t>new Error("SNMP Error")</t>
+  </si>
+  <si>
+    <t>return 'Failed to send email'</t>
+  </si>
+  <si>
+    <t>return Error แต่ไม่ใช่ 'Failed to send email'</t>
+  </si>
+  <si>
+    <t>ทดสอบฟังก์ชันการส่งอีเมลใน services</t>
+  </si>
+  <si>
+    <t>เปิดหน้าต่างการลบ</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1. เข้าเว็บไซต์ Painamnae                       2. Login                                              3. เข้าหน้าบัญชีของฉัน                            4. กดปุ่มลบข้อมูลบัญชี</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>username, password</t>
+  </si>
+  <si>
+    <t>แสดงหน้า 'เลือกข้อมูลที่คุณต้องการจะลบ'</t>
+  </si>
+  <si>
+    <t>ผู้ใช้ลบข้อมูลทุกอย่างในบัญชี</t>
+  </si>
+  <si>
+    <t>ผู้ใช้ลบเฉพาะข้อมูลยานพาหนะ</t>
+  </si>
+  <si>
+    <t>ข้อมูลการจองต้องไม่หาย</t>
+  </si>
+  <si>
+    <t>ผู้ใช้รับข้อมูลทางอีเมล</t>
+  </si>
+  <si>
+    <t>ผู้ใช้ยกเลิกการลบบัญชี</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1. เข้าเว็บไซต์ Painamnae                       2. Login                                              3. เข้าหน้าบัญชีของฉัน                            4. กดปุ่มลบข้อมูลบัญชี                            5. เลือกลบเฉพาะข้อมูลยานพาหนะ            6. กดยืนยันการลบ</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1. เข้าเว็บไซต์ Painamnae                       2. Login                                              3. เข้าหน้าบัญชีของฉัน                            4. กดปุ่มลบข้อมูลบัญชี                            5. เลือกลบข้อมูลบัญชี                              6. กดยืนยันการลบ</t>
+  </si>
+  <si>
+    <t>ข้อมูลทุกอย่างถูกลบและไม่สามารถ Login ได้</t>
+  </si>
+  <si>
+    <t>ข้อมูลบัญชีและยานพาหนะถูกลบและไม่สามารถ Login ได้</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1. เข้าเว็บไซต์ Painamnae                       2. Login                                              3. เข้าหน้าบัญชีของฉัน                            4. กดปุ่มลบข้อมูลบัญชี                            5. เลือกลบข้อมูลบัญชี                              6. เลือกส่งข้อมูลมาที่อีเมล</t>
+  </si>
+  <si>
+    <t>ข้อมูลทุกอย่างถูกลบและมีการส่งข้อมูลไปทางอีเมล</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1. เข้าเว็บไซต์ Painamnae                       2. Login                                              3. จองการเดินทาง                                  4. เข้าหน้าบัญชีของฉัน                            5. กดปุ่มลบข้อมูลบัญชี                            6. เลือกลบเฉพาะข้อมูลยานพาหนะ            7. กดยืนยันการลบ</t>
+  </si>
+  <si>
+    <t>ชื่อผู้ใช้ในการเข้าสู่ระบบ</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>รหัสผ่านผู้ใช้ในการเข้าสู่ระบบ</t>
+  </si>
+  <si>
+    <t>tester</t>
+  </si>
+  <si>
+    <t>tester555</t>
+  </si>
+  <si>
+    <t>ออกจากหน้าต่างยืนยัน</t>
+  </si>
+  <si>
+    <t>ข้อมูลที่เคยจองยังไม่หาย</t>
+  </si>
+  <si>
+    <t>API สำหรับการลบ</t>
+  </si>
+  <si>
+    <t>API การลบ Account</t>
   </si>
 </sst>
 </file>
@@ -383,7 +627,7 @@
   <numFmts count="1">
     <numFmt numFmtId="187" formatCode="0.0"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -446,6 +690,24 @@
     <font>
       <sz val="16"/>
       <color theme="1"/>
+      <name val="TH SarabunPSK"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF00B050"/>
+      <name val="TH SarabunPSK"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FFFF0000"/>
       <name val="TH SarabunPSK"/>
       <family val="2"/>
     </font>
@@ -696,7 +958,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="105">
+  <cellXfs count="129">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -764,9 +1026,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -775,13 +1034,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -794,9 +1046,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -842,6 +1091,105 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="187" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -860,9 +1208,6 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -884,107 +1229,88 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="187" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -5488,7 +5814,7 @@
   <dimension ref="A2:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="24" x14ac:dyDescent="0.55000000000000004"/>
@@ -5541,7 +5867,7 @@
         <v>9</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
@@ -5554,9 +5880,11 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="6"/>
-      <c r="B4" s="6"/>
+      <c r="B4" s="5" t="s">
+        <v>114</v>
+      </c>
       <c r="C4" s="5" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
@@ -5567,8 +5895,12 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
+      <c r="B5" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>107</v>
+      </c>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
@@ -5578,8 +5910,12 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="6"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
+      <c r="B6" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>187</v>
+      </c>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
@@ -5599,11 +5935,11 @@
       <c r="I7" s="6"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="42" t="s">
+      <c r="A8" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="43"/>
-      <c r="C8" s="44"/>
+      <c r="B8" s="38"/>
+      <c r="C8" s="39"/>
       <c r="D8" s="6"/>
       <c r="E8" s="10"/>
       <c r="F8" s="12"/>
@@ -5617,6 +5953,7 @@
   <mergeCells count="1">
     <mergeCell ref="A8:C8"/>
   </mergeCells>
+  <phoneticPr fontId="10" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="I3" location="'TS001'!A1" display="TS001" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="I8" location="'Test Summary Report'!A1" display="Test Summary Report" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
@@ -5707,16 +6044,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32DB73B2-BC5F-B846-AC94-E47300653683}">
-  <dimension ref="A1:H29"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22.625" customWidth="1"/>
-    <col min="2" max="3" width="24.125" customWidth="1"/>
+    <col min="2" max="2" width="25.75" customWidth="1"/>
+    <col min="3" max="3" width="37.375" customWidth="1"/>
     <col min="4" max="4" width="15.875" customWidth="1"/>
     <col min="5" max="5" width="49.5" customWidth="1"/>
     <col min="6" max="6" width="28.375" customWidth="1"/>
@@ -5731,37 +6069,36 @@
       <c r="B1" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="23" t="s">
+      <c r="C1" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="24" t="s">
-        <v>109</v>
+      <c r="D1" s="24" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="24" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="B2" s="32" t="s">
-        <v>107</v>
-      </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="23" t="s">
+      <c r="B2" s="31" t="s">
+        <v>111</v>
+      </c>
+      <c r="C2" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="E2" s="24"/>
+      <c r="D2" s="24"/>
     </row>
     <row r="3" spans="1:8" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A3" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="23" t="s">
+      <c r="B3" s="24" t="s">
+        <v>113</v>
+      </c>
+      <c r="C3" s="23" t="s">
         <v>92</v>
       </c>
-      <c r="E3" s="24" t="s">
+      <c r="D3" s="24" t="s">
         <v>93</v>
       </c>
     </row>
@@ -5770,161 +6107,264 @@
         <v>94</v>
       </c>
       <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="23" t="s">
+      <c r="C4" s="23" t="s">
         <v>95</v>
       </c>
-      <c r="E4" s="24"/>
+      <c r="D4" s="128">
+        <v>244397</v>
+      </c>
     </row>
     <row r="5" spans="1:8" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A5" s="23" t="s">
         <v>96</v>
       </c>
-      <c r="B5" s="35"/>
-      <c r="C5" s="35"/>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
+      <c r="B5" s="100"/>
+      <c r="C5" s="101"/>
+      <c r="D5" s="102"/>
+      <c r="E5" s="103"/>
     </row>
     <row r="6" spans="1:8" ht="23.25" x14ac:dyDescent="0.2">
-      <c r="A6" s="23" t="s">
+      <c r="A6" s="105" t="s">
         <v>97</v>
       </c>
-      <c r="B6" s="36"/>
-      <c r="C6" s="36"/>
-      <c r="D6" s="36"/>
-      <c r="E6" s="36"/>
+      <c r="B6" s="106" t="s">
+        <v>153</v>
+      </c>
+      <c r="C6" s="107"/>
+      <c r="D6" s="108"/>
+      <c r="E6" s="104"/>
     </row>
     <row r="7" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A7" s="37" t="s">
+      <c r="A7" s="33" t="s">
         <v>98</v>
       </c>
-      <c r="B7" s="37"/>
-      <c r="C7" s="37"/>
-      <c r="D7" s="37"/>
-      <c r="E7" s="37"/>
-    </row>
-    <row r="8" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A8" s="25" t="s">
+      <c r="B7" s="33"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
+    </row>
+    <row r="8" spans="1:8" ht="23.25" x14ac:dyDescent="0.2">
+      <c r="A8" s="111" t="s">
+        <v>109</v>
+      </c>
+      <c r="B8" s="111" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="111" t="s">
         <v>110</v>
       </c>
-      <c r="B8" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="25"/>
-      <c r="D8" s="25" t="s">
+      <c r="D8" s="111" t="s">
         <v>34</v>
       </c>
-      <c r="E8" s="25" t="s">
+      <c r="E8" s="111" t="s">
         <v>99</v>
       </c>
-      <c r="F8" s="29" t="s">
+      <c r="F8" s="112" t="s">
         <v>101</v>
       </c>
-      <c r="G8" s="29" t="s">
+      <c r="G8" s="112" t="s">
         <v>13</v>
       </c>
-      <c r="H8" s="29" t="s">
+      <c r="H8" s="112" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A9" s="26"/>
-      <c r="B9" s="26"/>
-      <c r="C9" s="26"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="34"/>
-      <c r="F9" s="26"/>
-      <c r="G9" s="26"/>
-      <c r="H9" s="26"/>
-    </row>
-    <row r="10" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A10" s="26"/>
-      <c r="B10" s="26"/>
-      <c r="C10" s="26"/>
-      <c r="D10" s="26"/>
-      <c r="E10" s="26"/>
-      <c r="F10" s="26"/>
-      <c r="G10" s="26"/>
-      <c r="H10" s="26"/>
-    </row>
-    <row r="11" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A11" s="26"/>
-      <c r="B11" s="26"/>
-      <c r="C11" s="26"/>
-      <c r="D11" s="26"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="26"/>
-      <c r="H11" s="26"/>
-    </row>
-    <row r="12" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A12" s="26"/>
-      <c r="B12" s="26"/>
-      <c r="C12" s="26"/>
-      <c r="D12" s="26"/>
-      <c r="E12" s="26"/>
-      <c r="F12" s="26"/>
-      <c r="G12" s="26"/>
-      <c r="H12" s="26"/>
-    </row>
-    <row r="13" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A13" s="26"/>
-      <c r="B13" s="26"/>
-      <c r="C13" s="26"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="26"/>
-      <c r="F13" s="26"/>
-      <c r="G13" s="26"/>
-      <c r="H13" s="26"/>
-    </row>
-    <row r="14" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A14" s="26"/>
-      <c r="B14" s="26"/>
-      <c r="C14" s="26"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="26"/>
-      <c r="H14" s="26"/>
-    </row>
-    <row r="15" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A15" s="26"/>
-      <c r="B15" s="26"/>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="26"/>
-      <c r="G15" s="26"/>
-      <c r="H15" s="26"/>
-    </row>
-    <row r="16" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A16" s="26"/>
-      <c r="B16" s="26"/>
-      <c r="C16" s="26"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="26"/>
-      <c r="F16" s="26"/>
-      <c r="G16" s="26"/>
-      <c r="H16" s="26"/>
-    </row>
-    <row r="17" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A17" s="26"/>
-      <c r="B17" s="26"/>
-      <c r="C17" s="26"/>
-      <c r="D17" s="26"/>
-      <c r="E17" s="26"/>
-      <c r="F17" s="26"/>
-      <c r="G17" s="26"/>
-      <c r="H17" s="26"/>
+    <row r="9" spans="1:8" ht="139.5" x14ac:dyDescent="0.2">
+      <c r="A9" s="113" t="s">
+        <v>117</v>
+      </c>
+      <c r="B9" s="114" t="s">
+        <v>118</v>
+      </c>
+      <c r="C9" s="115" t="s">
+        <v>134</v>
+      </c>
+      <c r="D9" s="116" t="s">
+        <v>127</v>
+      </c>
+      <c r="E9" s="114" t="s">
+        <v>119</v>
+      </c>
+      <c r="F9" s="117" t="s">
+        <v>119</v>
+      </c>
+      <c r="G9" s="120" t="s">
+        <v>4</v>
+      </c>
+      <c r="H9" s="114"/>
+    </row>
+    <row r="10" spans="1:8" ht="93" x14ac:dyDescent="0.2">
+      <c r="A10" s="113" t="s">
+        <v>120</v>
+      </c>
+      <c r="B10" s="114" t="s">
+        <v>126</v>
+      </c>
+      <c r="C10" s="115" t="s">
+        <v>136</v>
+      </c>
+      <c r="D10" s="114" t="s">
+        <v>128</v>
+      </c>
+      <c r="E10" s="114" t="s">
+        <v>129</v>
+      </c>
+      <c r="F10" s="118" t="s">
+        <v>129</v>
+      </c>
+      <c r="G10" s="120" t="s">
+        <v>4</v>
+      </c>
+      <c r="H10" s="114"/>
+    </row>
+    <row r="11" spans="1:8" ht="93" x14ac:dyDescent="0.2">
+      <c r="A11" s="113" t="s">
+        <v>121</v>
+      </c>
+      <c r="B11" s="118" t="s">
+        <v>130</v>
+      </c>
+      <c r="C11" s="115" t="s">
+        <v>135</v>
+      </c>
+      <c r="D11" s="114" t="s">
+        <v>131</v>
+      </c>
+      <c r="E11" s="114" t="s">
+        <v>132</v>
+      </c>
+      <c r="F11" s="118" t="s">
+        <v>132</v>
+      </c>
+      <c r="G11" s="120" t="s">
+        <v>4</v>
+      </c>
+      <c r="H11" s="114"/>
+    </row>
+    <row r="12" spans="1:8" ht="93" x14ac:dyDescent="0.2">
+      <c r="A12" s="113" t="s">
+        <v>122</v>
+      </c>
+      <c r="B12" s="118" t="s">
+        <v>133</v>
+      </c>
+      <c r="C12" s="115" t="s">
+        <v>137</v>
+      </c>
+      <c r="D12" s="118" t="s">
+        <v>138</v>
+      </c>
+      <c r="E12" s="119" t="s">
+        <v>139</v>
+      </c>
+      <c r="F12" s="119" t="s">
+        <v>139</v>
+      </c>
+      <c r="G12" s="120" t="s">
+        <v>4</v>
+      </c>
+      <c r="H12" s="114"/>
+    </row>
+    <row r="13" spans="1:8" ht="93" x14ac:dyDescent="0.2">
+      <c r="A13" s="113" t="s">
+        <v>123</v>
+      </c>
+      <c r="B13" s="118" t="s">
+        <v>140</v>
+      </c>
+      <c r="C13" s="115" t="s">
+        <v>141</v>
+      </c>
+      <c r="D13" s="118" t="s">
+        <v>138</v>
+      </c>
+      <c r="E13" s="119" t="s">
+        <v>139</v>
+      </c>
+      <c r="F13" s="119" t="s">
+        <v>139</v>
+      </c>
+      <c r="G13" s="120" t="s">
+        <v>4</v>
+      </c>
+      <c r="H13" s="114"/>
+    </row>
+    <row r="14" spans="1:8" ht="93" x14ac:dyDescent="0.2">
+      <c r="A14" s="113" t="s">
+        <v>124</v>
+      </c>
+      <c r="B14" s="118" t="s">
+        <v>142</v>
+      </c>
+      <c r="C14" s="115" t="s">
+        <v>143</v>
+      </c>
+      <c r="D14" s="118" t="s">
+        <v>138</v>
+      </c>
+      <c r="E14" s="119" t="s">
+        <v>144</v>
+      </c>
+      <c r="F14" s="119" t="s">
+        <v>144</v>
+      </c>
+      <c r="G14" s="120" t="s">
+        <v>4</v>
+      </c>
+      <c r="H14" s="114"/>
+    </row>
+    <row r="15" spans="1:8" ht="93" x14ac:dyDescent="0.2">
+      <c r="A15" s="113" t="s">
+        <v>125</v>
+      </c>
+      <c r="B15" s="118" t="s">
+        <v>145</v>
+      </c>
+      <c r="C15" s="115" t="s">
+        <v>146</v>
+      </c>
+      <c r="D15" s="118" t="s">
+        <v>138</v>
+      </c>
+      <c r="E15" s="119" t="s">
+        <v>139</v>
+      </c>
+      <c r="F15" s="119" t="s">
+        <v>139</v>
+      </c>
+      <c r="G15" s="120" t="s">
+        <v>4</v>
+      </c>
+      <c r="H15" s="114"/>
+    </row>
+    <row r="16" spans="1:8" ht="23.25" x14ac:dyDescent="0.2">
+      <c r="A16" s="113"/>
+      <c r="B16" s="114"/>
+      <c r="C16" s="114"/>
+      <c r="D16" s="114"/>
+      <c r="E16" s="114"/>
+      <c r="F16" s="114"/>
+      <c r="G16" s="114"/>
+      <c r="H16" s="114"/>
+    </row>
+    <row r="17" spans="1:8" ht="23.25" x14ac:dyDescent="0.2">
+      <c r="A17" s="113"/>
+      <c r="B17" s="114"/>
+      <c r="C17" s="114"/>
+      <c r="D17" s="114"/>
+      <c r="E17" s="114"/>
+      <c r="F17" s="114"/>
+      <c r="G17" s="114"/>
+      <c r="H17" s="114"/>
     </row>
     <row r="18" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A18" s="27" t="s">
         <v>100</v>
       </c>
-      <c r="B18" s="38"/>
-      <c r="C18" s="39"/>
-      <c r="D18" s="39"/>
-      <c r="E18" s="40"/>
+      <c r="B18" s="34"/>
+      <c r="C18" s="35"/>
+      <c r="D18" s="35"/>
+      <c r="E18" s="36"/>
     </row>
     <row r="19" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A19" s="28"/>
@@ -5933,102 +6373,1271 @@
       <c r="D19" s="28"/>
       <c r="E19" s="28"/>
     </row>
-    <row r="20" spans="1:8" s="33" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A20" s="41" t="s">
+    <row r="20" spans="1:8" s="32" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A20" s="121" t="s">
         <v>102</v>
       </c>
-      <c r="B20" s="41"/>
-      <c r="C20" s="41"/>
-      <c r="D20" s="41"/>
-      <c r="E20" s="41"/>
-    </row>
-    <row r="21" spans="1:8" s="33" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B20" s="121"/>
+      <c r="C20" s="121"/>
+      <c r="D20" s="121"/>
+      <c r="E20" s="122"/>
+    </row>
+    <row r="21" spans="1:8" s="32" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A21" s="25" t="s">
         <v>103</v>
       </c>
       <c r="B21" s="25" t="s">
         <v>104</v>
       </c>
-      <c r="C21" s="25"/>
+      <c r="C21" s="25" t="s">
+        <v>10</v>
+      </c>
       <c r="D21" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="E21" s="25" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" s="33" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A22" s="26"/>
-      <c r="B22" s="26"/>
-      <c r="C22" s="26"/>
-      <c r="D22" s="26"/>
-      <c r="E22" s="26"/>
-    </row>
-    <row r="23" spans="1:8" s="33" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A23" s="26"/>
-      <c r="B23" s="26"/>
-      <c r="C23" s="26"/>
-      <c r="D23" s="26"/>
-      <c r="E23" s="26"/>
-    </row>
-    <row r="24" spans="1:8" s="33" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="E21" s="123"/>
+    </row>
+    <row r="22" spans="1:8" s="32" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A22" s="109">
+        <v>1</v>
+      </c>
+      <c r="B22" s="26" t="s">
+        <v>147</v>
+      </c>
+      <c r="C22" s="26" t="s">
+        <v>148</v>
+      </c>
+      <c r="D22" s="26" t="s">
+        <v>149</v>
+      </c>
+      <c r="E22" s="124"/>
+    </row>
+    <row r="23" spans="1:8" s="32" customFormat="1" ht="93" x14ac:dyDescent="0.35">
+      <c r="A23" s="113">
+        <v>2</v>
+      </c>
+      <c r="B23" s="114" t="s">
+        <v>150</v>
+      </c>
+      <c r="C23" s="114" t="s">
+        <v>151</v>
+      </c>
+      <c r="D23" s="110" t="s">
+        <v>152</v>
+      </c>
+      <c r="E23" s="124"/>
+    </row>
+    <row r="24" spans="1:8" s="32" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A24" s="26"/>
       <c r="B24" s="26"/>
       <c r="C24" s="26"/>
       <c r="D24" s="26"/>
-      <c r="E24" s="26"/>
-    </row>
-    <row r="25" spans="1:8" s="33" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="E24" s="124"/>
+    </row>
+    <row r="25" spans="1:8" s="32" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A25" s="26"/>
       <c r="B25" s="26"/>
       <c r="C25" s="26"/>
       <c r="D25" s="26"/>
-      <c r="E25" s="26"/>
-    </row>
-    <row r="26" spans="1:8" s="33" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="E25" s="124"/>
+    </row>
+    <row r="26" spans="1:8" s="32" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A26" s="26"/>
       <c r="B26" s="26"/>
       <c r="C26" s="26"/>
       <c r="D26" s="26"/>
-      <c r="E26" s="26"/>
-      <c r="F26" s="33" t="s">
+      <c r="E26" s="124"/>
+      <c r="F26" s="32" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="27" spans="1:8" s="33" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" s="32" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A27" s="26"/>
       <c r="B27" s="26"/>
       <c r="C27" s="26"/>
       <c r="D27" s="26"/>
-      <c r="E27" s="26"/>
-    </row>
-    <row r="28" spans="1:8" s="33" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="E27" s="124"/>
+    </row>
+    <row r="28" spans="1:8" s="32" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A28" s="26"/>
       <c r="B28" s="26"/>
       <c r="C28" s="26"/>
       <c r="D28" s="26"/>
-      <c r="E28" s="26"/>
-    </row>
-    <row r="29" spans="1:8" s="33" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="E28" s="124"/>
+    </row>
+    <row r="29" spans="1:8" s="32" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A29" s="26"/>
       <c r="B29" s="26"/>
       <c r="C29" s="26"/>
       <c r="D29" s="26"/>
-      <c r="E29" s="26"/>
+      <c r="E29" s="124"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E30" s="125"/>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
     <mergeCell ref="A7:E7"/>
     <mergeCell ref="B18:E18"/>
-    <mergeCell ref="A20:E20"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="A20:D20"/>
+  </mergeCells>
+  <phoneticPr fontId="10" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE70028B-F30F-4C77-9E14-49DB6D61ACF9}">
+  <dimension ref="A1:H30"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="22.625" customWidth="1"/>
+    <col min="2" max="2" width="25.75" customWidth="1"/>
+    <col min="3" max="3" width="37.375" customWidth="1"/>
+    <col min="4" max="4" width="30.875" customWidth="1"/>
+    <col min="5" max="5" width="49.5" customWidth="1"/>
+    <col min="6" max="6" width="28.375" customWidth="1"/>
+    <col min="7" max="7" width="25.875" customWidth="1"/>
+    <col min="8" max="8" width="30.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="23.25" x14ac:dyDescent="0.2">
+      <c r="A1" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>114</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="24" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="24" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="B2" s="31" t="s">
+        <v>112</v>
+      </c>
+      <c r="C2" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="D2" s="24"/>
+    </row>
+    <row r="3" spans="1:8" ht="23.25" x14ac:dyDescent="0.2">
+      <c r="A3" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>113</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="D3" s="24" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="23.25" x14ac:dyDescent="0.2">
+      <c r="A4" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="B4" s="24"/>
+      <c r="C4" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="D4" s="128">
+        <v>244397</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="23.25" x14ac:dyDescent="0.2">
+      <c r="A5" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="B5" s="100"/>
+      <c r="C5" s="101"/>
+      <c r="D5" s="102"/>
+      <c r="E5" s="103"/>
+    </row>
+    <row r="6" spans="1:8" ht="23.25" x14ac:dyDescent="0.2">
+      <c r="A6" s="105" t="s">
+        <v>97</v>
+      </c>
+      <c r="B6" s="106" t="s">
+        <v>162</v>
+      </c>
+      <c r="C6" s="107"/>
+      <c r="D6" s="108"/>
+      <c r="E6" s="104"/>
+    </row>
+    <row r="7" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A7" s="33" t="s">
+        <v>98</v>
+      </c>
+      <c r="B7" s="33"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
+    </row>
+    <row r="8" spans="1:8" ht="23.25" x14ac:dyDescent="0.2">
+      <c r="A8" s="111" t="s">
+        <v>109</v>
+      </c>
+      <c r="B8" s="111" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="111" t="s">
+        <v>110</v>
+      </c>
+      <c r="D8" s="111" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="111" t="s">
+        <v>99</v>
+      </c>
+      <c r="F8" s="112" t="s">
+        <v>101</v>
+      </c>
+      <c r="G8" s="112" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" s="112" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="93" x14ac:dyDescent="0.2">
+      <c r="A9" s="113" t="s">
+        <v>117</v>
+      </c>
+      <c r="B9" s="114" t="s">
+        <v>154</v>
+      </c>
+      <c r="C9" s="115" t="s">
+        <v>155</v>
+      </c>
+      <c r="D9" s="116" t="s">
+        <v>156</v>
+      </c>
+      <c r="E9" s="114" t="s">
+        <v>157</v>
+      </c>
+      <c r="F9" s="114" t="s">
+        <v>157</v>
+      </c>
+      <c r="G9" s="120" t="s">
+        <v>4</v>
+      </c>
+      <c r="H9" s="114"/>
+    </row>
+    <row r="10" spans="1:8" ht="93" x14ac:dyDescent="0.2">
+      <c r="A10" s="113" t="s">
+        <v>120</v>
+      </c>
+      <c r="B10" s="114" t="s">
+        <v>158</v>
+      </c>
+      <c r="C10" s="115" t="s">
+        <v>155</v>
+      </c>
+      <c r="D10" s="114" t="s">
+        <v>159</v>
+      </c>
+      <c r="E10" s="114" t="s">
+        <v>160</v>
+      </c>
+      <c r="F10" s="118" t="s">
+        <v>161</v>
+      </c>
+      <c r="G10" s="126" t="s">
+        <v>5</v>
+      </c>
+      <c r="H10" s="114"/>
+    </row>
+    <row r="11" spans="1:8" ht="23.25" x14ac:dyDescent="0.2">
+      <c r="A11" s="113"/>
+      <c r="B11" s="118"/>
+      <c r="C11" s="115"/>
+      <c r="D11" s="114"/>
+      <c r="E11" s="114"/>
+      <c r="F11" s="118"/>
+      <c r="G11" s="120"/>
+      <c r="H11" s="114"/>
+    </row>
+    <row r="12" spans="1:8" ht="23.25" x14ac:dyDescent="0.2">
+      <c r="A12" s="113"/>
+      <c r="B12" s="118"/>
+      <c r="C12" s="115"/>
+      <c r="D12" s="118"/>
+      <c r="E12" s="119"/>
+      <c r="F12" s="119"/>
+      <c r="G12" s="120"/>
+      <c r="H12" s="114"/>
+    </row>
+    <row r="13" spans="1:8" ht="23.25" x14ac:dyDescent="0.2">
+      <c r="A13" s="113"/>
+      <c r="B13" s="118"/>
+      <c r="C13" s="115"/>
+      <c r="D13" s="118"/>
+      <c r="E13" s="119"/>
+      <c r="F13" s="119"/>
+      <c r="G13" s="120"/>
+      <c r="H13" s="114"/>
+    </row>
+    <row r="14" spans="1:8" ht="23.25" x14ac:dyDescent="0.2">
+      <c r="A14" s="113"/>
+      <c r="B14" s="118"/>
+      <c r="C14" s="115"/>
+      <c r="D14" s="118"/>
+      <c r="E14" s="119"/>
+      <c r="F14" s="119"/>
+      <c r="G14" s="120"/>
+      <c r="H14" s="114"/>
+    </row>
+    <row r="15" spans="1:8" ht="23.25" x14ac:dyDescent="0.2">
+      <c r="A15" s="113"/>
+      <c r="B15" s="118"/>
+      <c r="C15" s="115"/>
+      <c r="D15" s="118"/>
+      <c r="E15" s="119"/>
+      <c r="F15" s="119"/>
+      <c r="G15" s="120"/>
+      <c r="H15" s="114"/>
+    </row>
+    <row r="16" spans="1:8" ht="23.25" x14ac:dyDescent="0.2">
+      <c r="A16" s="113"/>
+      <c r="B16" s="114"/>
+      <c r="C16" s="114"/>
+      <c r="D16" s="114"/>
+      <c r="E16" s="114"/>
+      <c r="F16" s="114"/>
+      <c r="G16" s="114"/>
+      <c r="H16" s="114"/>
+    </row>
+    <row r="17" spans="1:8" ht="23.25" x14ac:dyDescent="0.2">
+      <c r="A17" s="113"/>
+      <c r="B17" s="114"/>
+      <c r="C17" s="114"/>
+      <c r="D17" s="114"/>
+      <c r="E17" s="114"/>
+      <c r="F17" s="114"/>
+      <c r="G17" s="114"/>
+      <c r="H17" s="114"/>
+    </row>
+    <row r="18" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A18" s="27" t="s">
+        <v>100</v>
+      </c>
+      <c r="B18" s="34"/>
+      <c r="C18" s="35"/>
+      <c r="D18" s="35"/>
+      <c r="E18" s="36"/>
+    </row>
+    <row r="19" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A19" s="28"/>
+      <c r="B19" s="28"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="28"/>
+    </row>
+    <row r="20" spans="1:8" s="32" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A20" s="121" t="s">
+        <v>102</v>
+      </c>
+      <c r="B20" s="121"/>
+      <c r="C20" s="121"/>
+      <c r="D20" s="121"/>
+      <c r="E20" s="122"/>
+    </row>
+    <row r="21" spans="1:8" s="32" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A21" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="B21" s="25" t="s">
+        <v>104</v>
+      </c>
+      <c r="C21" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="E21" s="123"/>
+    </row>
+    <row r="22" spans="1:8" s="32" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A22" s="109"/>
+      <c r="B22" s="26"/>
+      <c r="C22" s="26"/>
+      <c r="D22" s="26"/>
+      <c r="E22" s="124"/>
+    </row>
+    <row r="23" spans="1:8" s="32" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A23" s="113"/>
+      <c r="B23" s="114"/>
+      <c r="C23" s="114"/>
+      <c r="D23" s="110"/>
+      <c r="E23" s="124"/>
+    </row>
+    <row r="24" spans="1:8" s="32" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A24" s="26"/>
+      <c r="B24" s="26"/>
+      <c r="C24" s="26"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="124"/>
+    </row>
+    <row r="25" spans="1:8" s="32" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A25" s="26"/>
+      <c r="B25" s="26"/>
+      <c r="C25" s="26"/>
+      <c r="D25" s="26"/>
+      <c r="E25" s="124"/>
+    </row>
+    <row r="26" spans="1:8" s="32" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A26" s="26"/>
+      <c r="B26" s="26"/>
+      <c r="C26" s="26"/>
+      <c r="D26" s="26"/>
+      <c r="E26" s="124"/>
+      <c r="F26" s="32" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" s="32" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A27" s="26"/>
+      <c r="B27" s="26"/>
+      <c r="C27" s="26"/>
+      <c r="D27" s="26"/>
+      <c r="E27" s="124"/>
+    </row>
+    <row r="28" spans="1:8" s="32" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A28" s="26"/>
+      <c r="B28" s="26"/>
+      <c r="C28" s="26"/>
+      <c r="D28" s="26"/>
+      <c r="E28" s="124"/>
+    </row>
+    <row r="29" spans="1:8" s="32" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A29" s="26"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="124"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E30" s="125"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="A7:E7"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="A20:D20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FC1DBA5-9716-465D-A69E-ABAD665D625E}">
+  <dimension ref="A1:H30"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="22.625" customWidth="1"/>
+    <col min="2" max="2" width="25.75" customWidth="1"/>
+    <col min="3" max="3" width="37.375" customWidth="1"/>
+    <col min="4" max="4" width="30.875" customWidth="1"/>
+    <col min="5" max="5" width="49.5" customWidth="1"/>
+    <col min="6" max="6" width="42" customWidth="1"/>
+    <col min="7" max="7" width="25.875" customWidth="1"/>
+    <col min="8" max="8" width="30.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="23.25" x14ac:dyDescent="0.2">
+      <c r="A1" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>115</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="24" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="24" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="B2" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="C2" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="D2" s="24"/>
+    </row>
+    <row r="3" spans="1:8" ht="23.25" x14ac:dyDescent="0.2">
+      <c r="A3" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>113</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="D3" s="24" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="23.25" x14ac:dyDescent="0.2">
+      <c r="A4" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="B4" s="24"/>
+      <c r="C4" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="D4" s="128">
+        <v>244397</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="23.25" x14ac:dyDescent="0.2">
+      <c r="A5" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="B5" s="100"/>
+      <c r="C5" s="101"/>
+      <c r="D5" s="102"/>
+      <c r="E5" s="103"/>
+    </row>
+    <row r="6" spans="1:8" ht="23.25" x14ac:dyDescent="0.2">
+      <c r="A6" s="105" t="s">
+        <v>97</v>
+      </c>
+      <c r="B6" s="106" t="s">
+        <v>162</v>
+      </c>
+      <c r="C6" s="107"/>
+      <c r="D6" s="108"/>
+      <c r="E6" s="104"/>
+    </row>
+    <row r="7" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A7" s="33" t="s">
+        <v>98</v>
+      </c>
+      <c r="B7" s="33"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
+    </row>
+    <row r="8" spans="1:8" ht="23.25" x14ac:dyDescent="0.2">
+      <c r="A8" s="111" t="s">
+        <v>109</v>
+      </c>
+      <c r="B8" s="111" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="111" t="s">
+        <v>110</v>
+      </c>
+      <c r="D8" s="111" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="111" t="s">
+        <v>99</v>
+      </c>
+      <c r="F8" s="112" t="s">
+        <v>101</v>
+      </c>
+      <c r="G8" s="112" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" s="112" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="93" x14ac:dyDescent="0.2">
+      <c r="A9" s="113" t="s">
+        <v>117</v>
+      </c>
+      <c r="B9" s="114" t="s">
+        <v>163</v>
+      </c>
+      <c r="C9" s="115" t="s">
+        <v>164</v>
+      </c>
+      <c r="D9" s="116" t="s">
+        <v>166</v>
+      </c>
+      <c r="E9" s="114" t="s">
+        <v>167</v>
+      </c>
+      <c r="F9" s="114" t="s">
+        <v>167</v>
+      </c>
+      <c r="G9" s="120" t="s">
+        <v>4</v>
+      </c>
+      <c r="H9" s="114"/>
+    </row>
+    <row r="10" spans="1:8" ht="139.5" x14ac:dyDescent="0.2">
+      <c r="A10" s="113" t="s">
+        <v>120</v>
+      </c>
+      <c r="B10" s="114" t="s">
+        <v>168</v>
+      </c>
+      <c r="C10" s="115" t="s">
+        <v>174</v>
+      </c>
+      <c r="D10" s="116" t="s">
+        <v>166</v>
+      </c>
+      <c r="E10" s="114" t="s">
+        <v>175</v>
+      </c>
+      <c r="F10" s="114" t="s">
+        <v>175</v>
+      </c>
+      <c r="G10" s="120" t="s">
+        <v>4</v>
+      </c>
+      <c r="H10" s="114"/>
+    </row>
+    <row r="11" spans="1:8" ht="139.5" x14ac:dyDescent="0.2">
+      <c r="A11" s="113" t="s">
+        <v>121</v>
+      </c>
+      <c r="B11" s="118" t="s">
+        <v>169</v>
+      </c>
+      <c r="C11" s="115" t="s">
+        <v>173</v>
+      </c>
+      <c r="D11" s="116" t="s">
+        <v>166</v>
+      </c>
+      <c r="E11" s="114" t="s">
+        <v>176</v>
+      </c>
+      <c r="F11" s="114" t="s">
+        <v>176</v>
+      </c>
+      <c r="G11" s="120" t="s">
+        <v>4</v>
+      </c>
+      <c r="H11" s="114"/>
+    </row>
+    <row r="12" spans="1:8" ht="162.75" x14ac:dyDescent="0.2">
+      <c r="A12" s="113" t="s">
+        <v>122</v>
+      </c>
+      <c r="B12" s="118" t="s">
+        <v>170</v>
+      </c>
+      <c r="C12" s="115" t="s">
+        <v>179</v>
+      </c>
+      <c r="D12" s="116" t="s">
+        <v>166</v>
+      </c>
+      <c r="E12" s="119" t="s">
+        <v>186</v>
+      </c>
+      <c r="F12" s="119" t="s">
+        <v>186</v>
+      </c>
+      <c r="G12" s="120" t="s">
+        <v>4</v>
+      </c>
+      <c r="H12" s="114"/>
+    </row>
+    <row r="13" spans="1:8" ht="139.5" x14ac:dyDescent="0.2">
+      <c r="A13" s="113" t="s">
+        <v>123</v>
+      </c>
+      <c r="B13" s="118" t="s">
+        <v>171</v>
+      </c>
+      <c r="C13" s="115" t="s">
+        <v>177</v>
+      </c>
+      <c r="D13" s="116" t="s">
+        <v>166</v>
+      </c>
+      <c r="E13" s="114" t="s">
+        <v>178</v>
+      </c>
+      <c r="F13" s="114" t="s">
+        <v>178</v>
+      </c>
+      <c r="G13" s="120" t="s">
+        <v>4</v>
+      </c>
+      <c r="H13" s="114"/>
+    </row>
+    <row r="14" spans="1:8" ht="139.5" x14ac:dyDescent="0.2">
+      <c r="A14" s="113" t="s">
+        <v>124</v>
+      </c>
+      <c r="B14" s="118" t="s">
+        <v>172</v>
+      </c>
+      <c r="C14" s="115" t="s">
+        <v>177</v>
+      </c>
+      <c r="D14" s="118" t="s">
+        <v>166</v>
+      </c>
+      <c r="E14" s="119" t="s">
+        <v>185</v>
+      </c>
+      <c r="F14" s="119" t="s">
+        <v>185</v>
+      </c>
+      <c r="G14" s="120" t="s">
+        <v>4</v>
+      </c>
+      <c r="H14" s="114"/>
+    </row>
+    <row r="15" spans="1:8" ht="23.25" x14ac:dyDescent="0.2">
+      <c r="A15" s="113"/>
+      <c r="B15" s="118"/>
+      <c r="C15" s="127"/>
+      <c r="E15" s="119"/>
+      <c r="F15" s="119"/>
+      <c r="G15" s="120"/>
+      <c r="H15" s="114"/>
+    </row>
+    <row r="16" spans="1:8" ht="23.25" x14ac:dyDescent="0.2">
+      <c r="A16" s="113"/>
+      <c r="B16" s="114"/>
+      <c r="C16" s="114"/>
+      <c r="D16" s="114"/>
+      <c r="E16" s="114"/>
+      <c r="F16" s="114"/>
+      <c r="G16" s="114"/>
+      <c r="H16" s="114"/>
+    </row>
+    <row r="17" spans="1:8" ht="23.25" x14ac:dyDescent="0.2">
+      <c r="A17" s="113"/>
+      <c r="B17" s="114"/>
+      <c r="C17" s="114"/>
+      <c r="D17" s="114"/>
+      <c r="E17" s="114"/>
+      <c r="F17" s="114"/>
+      <c r="G17" s="114"/>
+      <c r="H17" s="114"/>
+    </row>
+    <row r="18" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A18" s="27" t="s">
+        <v>100</v>
+      </c>
+      <c r="B18" s="34"/>
+      <c r="C18" s="35"/>
+      <c r="D18" s="35"/>
+      <c r="E18" s="36"/>
+    </row>
+    <row r="19" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A19" s="28"/>
+      <c r="B19" s="28"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="28"/>
+    </row>
+    <row r="20" spans="1:8" s="32" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A20" s="121" t="s">
+        <v>102</v>
+      </c>
+      <c r="B20" s="121"/>
+      <c r="C20" s="121"/>
+      <c r="D20" s="121"/>
+      <c r="E20" s="122"/>
+    </row>
+    <row r="21" spans="1:8" s="32" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A21" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="B21" s="25" t="s">
+        <v>104</v>
+      </c>
+      <c r="C21" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="E21" s="123"/>
+    </row>
+    <row r="22" spans="1:8" s="32" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A22" s="109">
+        <v>1</v>
+      </c>
+      <c r="B22" s="26" t="s">
+        <v>165</v>
+      </c>
+      <c r="C22" s="26" t="s">
+        <v>180</v>
+      </c>
+      <c r="D22" s="26" t="s">
+        <v>183</v>
+      </c>
+      <c r="E22" s="124"/>
+    </row>
+    <row r="23" spans="1:8" s="32" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A23" s="113">
+        <v>2</v>
+      </c>
+      <c r="B23" s="114" t="s">
+        <v>181</v>
+      </c>
+      <c r="C23" s="26" t="s">
+        <v>182</v>
+      </c>
+      <c r="D23" s="110" t="s">
+        <v>184</v>
+      </c>
+      <c r="E23" s="124"/>
+    </row>
+    <row r="24" spans="1:8" s="32" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A24" s="26"/>
+      <c r="B24" s="26"/>
+      <c r="C24" s="26"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="124"/>
+    </row>
+    <row r="25" spans="1:8" s="32" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A25" s="26"/>
+      <c r="B25" s="26"/>
+      <c r="C25" s="26"/>
+      <c r="D25" s="26"/>
+      <c r="E25" s="124"/>
+    </row>
+    <row r="26" spans="1:8" s="32" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A26" s="26"/>
+      <c r="B26" s="26"/>
+      <c r="C26" s="26"/>
+      <c r="D26" s="26"/>
+      <c r="E26" s="124"/>
+      <c r="F26" s="32" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" s="32" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A27" s="26"/>
+      <c r="B27" s="26"/>
+      <c r="C27" s="26"/>
+      <c r="D27" s="26"/>
+      <c r="E27" s="124"/>
+    </row>
+    <row r="28" spans="1:8" s="32" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A28" s="26"/>
+      <c r="B28" s="26"/>
+      <c r="C28" s="26"/>
+      <c r="D28" s="26"/>
+      <c r="E28" s="124"/>
+    </row>
+    <row r="29" spans="1:8" s="32" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A29" s="26"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="124"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E30" s="125"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="A7:E7"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="A20:D20"/>
+  </mergeCells>
+  <phoneticPr fontId="10" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F28B651-36A1-410B-AA5C-FB1ED4CA5D53}">
+  <dimension ref="A1:H30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="22.625" customWidth="1"/>
+    <col min="2" max="2" width="25.75" customWidth="1"/>
+    <col min="3" max="3" width="37.375" customWidth="1"/>
+    <col min="4" max="4" width="30.875" customWidth="1"/>
+    <col min="5" max="5" width="49.5" customWidth="1"/>
+    <col min="6" max="6" width="28.375" customWidth="1"/>
+    <col min="7" max="7" width="25.875" customWidth="1"/>
+    <col min="8" max="8" width="30.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="23.25" x14ac:dyDescent="0.2">
+      <c r="A1" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>116</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="24" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="24" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="B2" s="31" t="s">
+        <v>188</v>
+      </c>
+      <c r="C2" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="D2" s="24"/>
+    </row>
+    <row r="3" spans="1:8" ht="23.25" x14ac:dyDescent="0.2">
+      <c r="A3" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>113</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="D3" s="24" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="23.25" x14ac:dyDescent="0.2">
+      <c r="A4" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="B4" s="24"/>
+      <c r="C4" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="D4" s="128">
+        <v>244397</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="23.25" x14ac:dyDescent="0.2">
+      <c r="A5" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="B5" s="100"/>
+      <c r="C5" s="101"/>
+      <c r="D5" s="102"/>
+      <c r="E5" s="103"/>
+    </row>
+    <row r="6" spans="1:8" ht="23.25" x14ac:dyDescent="0.2">
+      <c r="A6" s="105" t="s">
+        <v>97</v>
+      </c>
+      <c r="B6" s="106" t="s">
+        <v>162</v>
+      </c>
+      <c r="C6" s="107"/>
+      <c r="D6" s="108"/>
+      <c r="E6" s="104"/>
+    </row>
+    <row r="7" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A7" s="33" t="s">
+        <v>98</v>
+      </c>
+      <c r="B7" s="33"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
+    </row>
+    <row r="8" spans="1:8" ht="23.25" x14ac:dyDescent="0.2">
+      <c r="A8" s="111" t="s">
+        <v>109</v>
+      </c>
+      <c r="B8" s="111" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="111" t="s">
+        <v>110</v>
+      </c>
+      <c r="D8" s="111" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="111" t="s">
+        <v>99</v>
+      </c>
+      <c r="F8" s="112" t="s">
+        <v>101</v>
+      </c>
+      <c r="G8" s="112" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" s="112" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="93" x14ac:dyDescent="0.2">
+      <c r="A9" s="113" t="s">
+        <v>117</v>
+      </c>
+      <c r="B9" s="114" t="s">
+        <v>154</v>
+      </c>
+      <c r="C9" s="115" t="s">
+        <v>155</v>
+      </c>
+      <c r="D9" s="116" t="s">
+        <v>156</v>
+      </c>
+      <c r="E9" s="114" t="s">
+        <v>157</v>
+      </c>
+      <c r="F9" s="114" t="s">
+        <v>157</v>
+      </c>
+      <c r="G9" s="120" t="s">
+        <v>4</v>
+      </c>
+      <c r="H9" s="114"/>
+    </row>
+    <row r="10" spans="1:8" ht="93" x14ac:dyDescent="0.2">
+      <c r="A10" s="113" t="s">
+        <v>120</v>
+      </c>
+      <c r="B10" s="114" t="s">
+        <v>158</v>
+      </c>
+      <c r="C10" s="115" t="s">
+        <v>155</v>
+      </c>
+      <c r="D10" s="114" t="s">
+        <v>159</v>
+      </c>
+      <c r="E10" s="114" t="s">
+        <v>160</v>
+      </c>
+      <c r="F10" s="118" t="s">
+        <v>161</v>
+      </c>
+      <c r="G10" s="126" t="s">
+        <v>5</v>
+      </c>
+      <c r="H10" s="114"/>
+    </row>
+    <row r="11" spans="1:8" ht="23.25" x14ac:dyDescent="0.2">
+      <c r="A11" s="113"/>
+      <c r="B11" s="118"/>
+      <c r="C11" s="115"/>
+      <c r="D11" s="114"/>
+      <c r="E11" s="114"/>
+      <c r="F11" s="118"/>
+      <c r="G11" s="120"/>
+      <c r="H11" s="114"/>
+    </row>
+    <row r="12" spans="1:8" ht="23.25" x14ac:dyDescent="0.2">
+      <c r="A12" s="113"/>
+      <c r="B12" s="118"/>
+      <c r="C12" s="115"/>
+      <c r="D12" s="118"/>
+      <c r="E12" s="119"/>
+      <c r="F12" s="119"/>
+      <c r="G12" s="120"/>
+      <c r="H12" s="114"/>
+    </row>
+    <row r="13" spans="1:8" ht="23.25" x14ac:dyDescent="0.2">
+      <c r="A13" s="113"/>
+      <c r="B13" s="118"/>
+      <c r="C13" s="115"/>
+      <c r="D13" s="118"/>
+      <c r="E13" s="119"/>
+      <c r="F13" s="119"/>
+      <c r="G13" s="120"/>
+      <c r="H13" s="114"/>
+    </row>
+    <row r="14" spans="1:8" ht="23.25" x14ac:dyDescent="0.2">
+      <c r="A14" s="113"/>
+      <c r="B14" s="118"/>
+      <c r="C14" s="115"/>
+      <c r="D14" s="118"/>
+      <c r="E14" s="119"/>
+      <c r="F14" s="119"/>
+      <c r="G14" s="120"/>
+      <c r="H14" s="114"/>
+    </row>
+    <row r="15" spans="1:8" ht="23.25" x14ac:dyDescent="0.2">
+      <c r="A15" s="113"/>
+      <c r="B15" s="118"/>
+      <c r="C15" s="115"/>
+      <c r="D15" s="118"/>
+      <c r="E15" s="119"/>
+      <c r="F15" s="119"/>
+      <c r="G15" s="120"/>
+      <c r="H15" s="114"/>
+    </row>
+    <row r="16" spans="1:8" ht="23.25" x14ac:dyDescent="0.2">
+      <c r="A16" s="113"/>
+      <c r="B16" s="114"/>
+      <c r="C16" s="114"/>
+      <c r="D16" s="114"/>
+      <c r="E16" s="114"/>
+      <c r="F16" s="114"/>
+      <c r="G16" s="114"/>
+      <c r="H16" s="114"/>
+    </row>
+    <row r="17" spans="1:8" ht="23.25" x14ac:dyDescent="0.2">
+      <c r="A17" s="113"/>
+      <c r="B17" s="114"/>
+      <c r="C17" s="114"/>
+      <c r="D17" s="114"/>
+      <c r="E17" s="114"/>
+      <c r="F17" s="114"/>
+      <c r="G17" s="114"/>
+      <c r="H17" s="114"/>
+    </row>
+    <row r="18" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A18" s="27" t="s">
+        <v>100</v>
+      </c>
+      <c r="B18" s="34"/>
+      <c r="C18" s="35"/>
+      <c r="D18" s="35"/>
+      <c r="E18" s="36"/>
+    </row>
+    <row r="19" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A19" s="28"/>
+      <c r="B19" s="28"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="28"/>
+    </row>
+    <row r="20" spans="1:8" s="32" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A20" s="121" t="s">
+        <v>102</v>
+      </c>
+      <c r="B20" s="121"/>
+      <c r="C20" s="121"/>
+      <c r="D20" s="121"/>
+      <c r="E20" s="122"/>
+    </row>
+    <row r="21" spans="1:8" s="32" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A21" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="B21" s="25" t="s">
+        <v>104</v>
+      </c>
+      <c r="C21" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="E21" s="123"/>
+    </row>
+    <row r="22" spans="1:8" s="32" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A22" s="109"/>
+      <c r="B22" s="26"/>
+      <c r="C22" s="26"/>
+      <c r="D22" s="26"/>
+      <c r="E22" s="124"/>
+    </row>
+    <row r="23" spans="1:8" s="32" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A23" s="113"/>
+      <c r="B23" s="114"/>
+      <c r="C23" s="114"/>
+      <c r="D23" s="110"/>
+      <c r="E23" s="124"/>
+    </row>
+    <row r="24" spans="1:8" s="32" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A24" s="26"/>
+      <c r="B24" s="26"/>
+      <c r="C24" s="26"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="124"/>
+    </row>
+    <row r="25" spans="1:8" s="32" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A25" s="26"/>
+      <c r="B25" s="26"/>
+      <c r="C25" s="26"/>
+      <c r="D25" s="26"/>
+      <c r="E25" s="124"/>
+    </row>
+    <row r="26" spans="1:8" s="32" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A26" s="26"/>
+      <c r="B26" s="26"/>
+      <c r="C26" s="26"/>
+      <c r="D26" s="26"/>
+      <c r="E26" s="124"/>
+      <c r="F26" s="32" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" s="32" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A27" s="26"/>
+      <c r="B27" s="26"/>
+      <c r="C27" s="26"/>
+      <c r="D27" s="26"/>
+      <c r="E27" s="124"/>
+    </row>
+    <row r="28" spans="1:8" s="32" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A28" s="26"/>
+      <c r="B28" s="26"/>
+      <c r="C28" s="26"/>
+      <c r="D28" s="26"/>
+      <c r="E28" s="124"/>
+    </row>
+    <row r="29" spans="1:8" s="32" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A29" s="26"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="124"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E30" s="125"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="A7:E7"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="A20:D20"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A2:F12"/>
   <sheetViews>
@@ -6051,50 +7660,50 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
+      <c r="B2" s="40"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="B4" s="49"/>
-      <c r="C4" s="50"/>
+      <c r="B4" s="44"/>
+      <c r="C4" s="45"/>
       <c r="D4" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="E4" s="49"/>
-      <c r="F4" s="51"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="46"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="B5" s="49"/>
-      <c r="C5" s="50"/>
+      <c r="B5" s="44"/>
+      <c r="C5" s="45"/>
       <c r="D5" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="E5" s="52"/>
-      <c r="F5" s="53"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="48"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="31" t="s">
+      <c r="A6" s="30" t="s">
         <v>80</v>
       </c>
-      <c r="B6" s="54"/>
-      <c r="C6" s="55"/>
-      <c r="D6" s="55"/>
-      <c r="E6" s="55"/>
-      <c r="F6" s="56"/>
-    </row>
-    <row r="8" spans="1:6" s="30" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="49"/>
+      <c r="C6" s="50"/>
+      <c r="D6" s="50"/>
+      <c r="E6" s="50"/>
+      <c r="F6" s="51"/>
+    </row>
+    <row r="8" spans="1:6" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
         <v>0</v>
       </c>
@@ -6115,7 +7724,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="46" t="s">
+      <c r="A9" s="41" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="6" t="s">
@@ -6127,7 +7736,7 @@
       <c r="F9" s="6"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="47"/>
+      <c r="A10" s="42"/>
       <c r="B10" s="6" t="s">
         <v>87</v>
       </c>
@@ -6137,7 +7746,7 @@
       <c r="F10" s="6"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="47"/>
+      <c r="A11" s="42"/>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
@@ -6145,7 +7754,7 @@
       <c r="F11" s="6"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="48"/>
+      <c r="A12" s="43"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
@@ -6167,7 +7776,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A2:AD37"/>
   <sheetViews>
@@ -6189,771 +7798,771 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:30" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="101" t="s">
+      <c r="A2" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="101"/>
-      <c r="C2" s="101"/>
-      <c r="D2" s="101"/>
-      <c r="E2" s="101"/>
-      <c r="F2" s="101"/>
-      <c r="G2" s="101"/>
-      <c r="H2" s="101"/>
-      <c r="I2" s="101"/>
-      <c r="J2" s="101"/>
-      <c r="K2" s="101"/>
+      <c r="B2" s="52"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="52"/>
+      <c r="J2" s="52"/>
+      <c r="K2" s="52"/>
     </row>
     <row r="3" spans="1:30" ht="24" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="104" t="s">
+      <c r="A3" s="56" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="104"/>
-      <c r="C3" s="104"/>
-      <c r="D3" s="71"/>
-      <c r="E3" s="71"/>
-      <c r="F3" s="71"/>
-      <c r="G3" s="71"/>
-      <c r="H3" s="71"/>
+      <c r="B3" s="56"/>
+      <c r="C3" s="56"/>
+      <c r="D3" s="57"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="57"/>
+      <c r="G3" s="57"/>
+      <c r="H3" s="57"/>
       <c r="I3" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="J3" s="103">
+      <c r="J3" s="55">
         <v>1</v>
       </c>
-      <c r="K3" s="103"/>
+      <c r="K3" s="55"/>
     </row>
     <row r="4" spans="1:30" ht="24" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="102" t="s">
+      <c r="A4" s="53" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="102"/>
-      <c r="C4" s="102"/>
-      <c r="D4" s="102"/>
-      <c r="E4" s="102"/>
-      <c r="F4" s="102"/>
-      <c r="G4" s="102"/>
-      <c r="H4" s="102"/>
-      <c r="I4" s="102"/>
-      <c r="J4" s="102"/>
-      <c r="K4" s="102"/>
-      <c r="M4" s="63" t="s">
+      <c r="B4" s="53"/>
+      <c r="C4" s="53"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="53"/>
+      <c r="F4" s="53"/>
+      <c r="G4" s="53"/>
+      <c r="H4" s="53"/>
+      <c r="I4" s="53"/>
+      <c r="J4" s="53"/>
+      <c r="K4" s="53"/>
+      <c r="M4" s="76" t="s">
         <v>79</v>
       </c>
-      <c r="N4" s="63"/>
-      <c r="O4" s="63"/>
-      <c r="P4" s="63"/>
-      <c r="Q4" s="63"/>
-      <c r="R4" s="63"/>
-      <c r="S4" s="63"/>
-      <c r="T4" s="63"/>
-      <c r="U4" s="63"/>
-      <c r="V4" s="63"/>
-      <c r="W4" s="63"/>
-      <c r="X4" s="63"/>
-      <c r="Y4" s="63"/>
-      <c r="Z4" s="63"/>
-      <c r="AA4" s="63"/>
-      <c r="AB4" s="63"/>
-      <c r="AC4" s="63"/>
-      <c r="AD4" s="63"/>
+      <c r="N4" s="76"/>
+      <c r="O4" s="76"/>
+      <c r="P4" s="76"/>
+      <c r="Q4" s="76"/>
+      <c r="R4" s="76"/>
+      <c r="S4" s="76"/>
+      <c r="T4" s="76"/>
+      <c r="U4" s="76"/>
+      <c r="V4" s="76"/>
+      <c r="W4" s="76"/>
+      <c r="X4" s="76"/>
+      <c r="Y4" s="76"/>
+      <c r="Z4" s="76"/>
+      <c r="AA4" s="76"/>
+      <c r="AB4" s="76"/>
+      <c r="AC4" s="76"/>
+      <c r="AD4" s="76"/>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="94" t="s">
+      <c r="A5" s="54" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="94"/>
-      <c r="C5" s="94"/>
-      <c r="D5" s="49"/>
-      <c r="E5" s="50"/>
-      <c r="F5" s="51"/>
-      <c r="G5" s="94" t="s">
+      <c r="B5" s="54"/>
+      <c r="C5" s="54"/>
+      <c r="D5" s="44"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="46"/>
+      <c r="G5" s="54" t="s">
         <v>20</v>
       </c>
-      <c r="H5" s="94"/>
-      <c r="I5" s="76"/>
-      <c r="J5" s="76"/>
-      <c r="K5" s="76"/>
-      <c r="M5" s="64"/>
-      <c r="N5" s="65"/>
-      <c r="O5" s="65"/>
-      <c r="P5" s="65"/>
-      <c r="Q5" s="65"/>
-      <c r="R5" s="65"/>
-      <c r="S5" s="65"/>
-      <c r="T5" s="65"/>
-      <c r="U5" s="65"/>
-      <c r="V5" s="65"/>
-      <c r="W5" s="65"/>
-      <c r="X5" s="65"/>
-      <c r="Y5" s="65"/>
-      <c r="Z5" s="65"/>
-      <c r="AA5" s="65"/>
-      <c r="AB5" s="65"/>
-      <c r="AC5" s="65"/>
-      <c r="AD5" s="66"/>
+      <c r="H5" s="54"/>
+      <c r="I5" s="59"/>
+      <c r="J5" s="59"/>
+      <c r="K5" s="59"/>
+      <c r="M5" s="91"/>
+      <c r="N5" s="92"/>
+      <c r="O5" s="92"/>
+      <c r="P5" s="92"/>
+      <c r="Q5" s="92"/>
+      <c r="R5" s="92"/>
+      <c r="S5" s="92"/>
+      <c r="T5" s="92"/>
+      <c r="U5" s="92"/>
+      <c r="V5" s="92"/>
+      <c r="W5" s="92"/>
+      <c r="X5" s="92"/>
+      <c r="Y5" s="92"/>
+      <c r="Z5" s="92"/>
+      <c r="AA5" s="92"/>
+      <c r="AB5" s="92"/>
+      <c r="AC5" s="92"/>
+      <c r="AD5" s="93"/>
     </row>
     <row r="6" spans="1:30" ht="24" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="94" t="s">
+      <c r="A6" s="54" t="s">
         <v>40</v>
       </c>
-      <c r="B6" s="94"/>
-      <c r="C6" s="94"/>
-      <c r="D6" s="49"/>
-      <c r="E6" s="50"/>
-      <c r="F6" s="51"/>
-      <c r="G6" s="94" t="s">
+      <c r="B6" s="54"/>
+      <c r="C6" s="54"/>
+      <c r="D6" s="44"/>
+      <c r="E6" s="45"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="54" t="s">
         <v>38</v>
       </c>
-      <c r="H6" s="94"/>
-      <c r="I6" s="49"/>
-      <c r="J6" s="50"/>
-      <c r="K6" s="51"/>
-      <c r="M6" s="67"/>
-      <c r="N6" s="68"/>
-      <c r="O6" s="68"/>
-      <c r="P6" s="68"/>
-      <c r="Q6" s="68"/>
-      <c r="R6" s="68"/>
-      <c r="S6" s="68"/>
-      <c r="T6" s="68"/>
-      <c r="U6" s="68"/>
-      <c r="V6" s="68"/>
-      <c r="W6" s="68"/>
-      <c r="X6" s="68"/>
-      <c r="Y6" s="68"/>
-      <c r="Z6" s="68"/>
-      <c r="AA6" s="68"/>
-      <c r="AB6" s="68"/>
-      <c r="AC6" s="68"/>
-      <c r="AD6" s="69"/>
+      <c r="H6" s="54"/>
+      <c r="I6" s="44"/>
+      <c r="J6" s="45"/>
+      <c r="K6" s="46"/>
+      <c r="M6" s="94"/>
+      <c r="N6" s="95"/>
+      <c r="O6" s="95"/>
+      <c r="P6" s="95"/>
+      <c r="Q6" s="95"/>
+      <c r="R6" s="95"/>
+      <c r="S6" s="95"/>
+      <c r="T6" s="95"/>
+      <c r="U6" s="95"/>
+      <c r="V6" s="95"/>
+      <c r="W6" s="95"/>
+      <c r="X6" s="95"/>
+      <c r="Y6" s="95"/>
+      <c r="Z6" s="95"/>
+      <c r="AA6" s="95"/>
+      <c r="AB6" s="95"/>
+      <c r="AC6" s="95"/>
+      <c r="AD6" s="96"/>
     </row>
     <row r="7" spans="1:30" ht="24" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="94" t="s">
+      <c r="A7" s="54" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="94"/>
-      <c r="C7" s="94"/>
-      <c r="D7" s="52"/>
-      <c r="E7" s="81"/>
-      <c r="F7" s="81"/>
-      <c r="G7" s="81"/>
-      <c r="H7" s="81"/>
-      <c r="I7" s="81"/>
-      <c r="J7" s="81"/>
-      <c r="K7" s="53"/>
-      <c r="M7" s="67"/>
-      <c r="N7" s="68"/>
-      <c r="O7" s="68"/>
-      <c r="P7" s="68"/>
-      <c r="Q7" s="68"/>
-      <c r="R7" s="68"/>
-      <c r="S7" s="68"/>
-      <c r="T7" s="68"/>
-      <c r="U7" s="68"/>
-      <c r="V7" s="68"/>
-      <c r="W7" s="68"/>
-      <c r="X7" s="68"/>
-      <c r="Y7" s="68"/>
-      <c r="Z7" s="68"/>
-      <c r="AA7" s="68"/>
-      <c r="AB7" s="68"/>
-      <c r="AC7" s="68"/>
-      <c r="AD7" s="69"/>
+      <c r="B7" s="54"/>
+      <c r="C7" s="54"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="58"/>
+      <c r="F7" s="58"/>
+      <c r="G7" s="58"/>
+      <c r="H7" s="58"/>
+      <c r="I7" s="58"/>
+      <c r="J7" s="58"/>
+      <c r="K7" s="48"/>
+      <c r="M7" s="94"/>
+      <c r="N7" s="95"/>
+      <c r="O7" s="95"/>
+      <c r="P7" s="95"/>
+      <c r="Q7" s="95"/>
+      <c r="R7" s="95"/>
+      <c r="S7" s="95"/>
+      <c r="T7" s="95"/>
+      <c r="U7" s="95"/>
+      <c r="V7" s="95"/>
+      <c r="W7" s="95"/>
+      <c r="X7" s="95"/>
+      <c r="Y7" s="95"/>
+      <c r="Z7" s="95"/>
+      <c r="AA7" s="95"/>
+      <c r="AB7" s="95"/>
+      <c r="AC7" s="95"/>
+      <c r="AD7" s="96"/>
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="94" t="s">
+      <c r="A8" s="54" t="s">
         <v>42</v>
       </c>
-      <c r="B8" s="94"/>
-      <c r="C8" s="94"/>
-      <c r="D8" s="94"/>
-      <c r="E8" s="94"/>
-      <c r="F8" s="94"/>
-      <c r="G8" s="94"/>
-      <c r="H8" s="94"/>
-      <c r="I8" s="94"/>
-      <c r="J8" s="94"/>
-      <c r="K8" s="94"/>
-      <c r="M8" s="67"/>
-      <c r="N8" s="68"/>
-      <c r="O8" s="68"/>
-      <c r="P8" s="68"/>
-      <c r="Q8" s="68"/>
-      <c r="R8" s="68"/>
-      <c r="S8" s="68"/>
-      <c r="T8" s="68"/>
-      <c r="U8" s="68"/>
-      <c r="V8" s="68"/>
-      <c r="W8" s="68"/>
-      <c r="X8" s="68"/>
-      <c r="Y8" s="68"/>
-      <c r="Z8" s="68"/>
-      <c r="AA8" s="68"/>
-      <c r="AB8" s="68"/>
-      <c r="AC8" s="68"/>
-      <c r="AD8" s="69"/>
+      <c r="B8" s="54"/>
+      <c r="C8" s="54"/>
+      <c r="D8" s="54"/>
+      <c r="E8" s="54"/>
+      <c r="F8" s="54"/>
+      <c r="G8" s="54"/>
+      <c r="H8" s="54"/>
+      <c r="I8" s="54"/>
+      <c r="J8" s="54"/>
+      <c r="K8" s="54"/>
+      <c r="M8" s="94"/>
+      <c r="N8" s="95"/>
+      <c r="O8" s="95"/>
+      <c r="P8" s="95"/>
+      <c r="Q8" s="95"/>
+      <c r="R8" s="95"/>
+      <c r="S8" s="95"/>
+      <c r="T8" s="95"/>
+      <c r="U8" s="95"/>
+      <c r="V8" s="95"/>
+      <c r="W8" s="95"/>
+      <c r="X8" s="95"/>
+      <c r="Y8" s="95"/>
+      <c r="Z8" s="95"/>
+      <c r="AA8" s="95"/>
+      <c r="AB8" s="95"/>
+      <c r="AC8" s="95"/>
+      <c r="AD8" s="96"/>
     </row>
     <row r="9" spans="1:30" ht="24" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="95" t="s">
+      <c r="A9" s="63" t="s">
         <v>43</v>
       </c>
-      <c r="B9" s="96"/>
-      <c r="C9" s="97"/>
-      <c r="D9" s="52">
+      <c r="B9" s="64"/>
+      <c r="C9" s="65"/>
+      <c r="D9" s="47">
         <v>1</v>
       </c>
-      <c r="E9" s="81"/>
-      <c r="F9" s="81"/>
-      <c r="G9" s="81"/>
-      <c r="H9" s="81"/>
-      <c r="I9" s="81"/>
-      <c r="J9" s="81"/>
-      <c r="K9" s="53"/>
-      <c r="M9" s="67"/>
-      <c r="N9" s="68"/>
-      <c r="O9" s="68"/>
-      <c r="P9" s="68"/>
-      <c r="Q9" s="68"/>
-      <c r="R9" s="68"/>
-      <c r="S9" s="68"/>
-      <c r="T9" s="68"/>
-      <c r="U9" s="68"/>
-      <c r="V9" s="68"/>
-      <c r="W9" s="68"/>
-      <c r="X9" s="68"/>
-      <c r="Y9" s="68"/>
-      <c r="Z9" s="68"/>
-      <c r="AA9" s="68"/>
-      <c r="AB9" s="68"/>
-      <c r="AC9" s="68"/>
-      <c r="AD9" s="69"/>
+      <c r="E9" s="58"/>
+      <c r="F9" s="58"/>
+      <c r="G9" s="58"/>
+      <c r="H9" s="58"/>
+      <c r="I9" s="58"/>
+      <c r="J9" s="58"/>
+      <c r="K9" s="48"/>
+      <c r="M9" s="94"/>
+      <c r="N9" s="95"/>
+      <c r="O9" s="95"/>
+      <c r="P9" s="95"/>
+      <c r="Q9" s="95"/>
+      <c r="R9" s="95"/>
+      <c r="S9" s="95"/>
+      <c r="T9" s="95"/>
+      <c r="U9" s="95"/>
+      <c r="V9" s="95"/>
+      <c r="W9" s="95"/>
+      <c r="X9" s="95"/>
+      <c r="Y9" s="95"/>
+      <c r="Z9" s="95"/>
+      <c r="AA9" s="95"/>
+      <c r="AB9" s="95"/>
+      <c r="AC9" s="95"/>
+      <c r="AD9" s="96"/>
     </row>
     <row r="10" spans="1:30" ht="24" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="98"/>
-      <c r="B10" s="99"/>
-      <c r="C10" s="100"/>
-      <c r="D10" s="52">
+      <c r="A10" s="66"/>
+      <c r="B10" s="67"/>
+      <c r="C10" s="68"/>
+      <c r="D10" s="47">
         <v>2</v>
       </c>
-      <c r="E10" s="81"/>
-      <c r="F10" s="81"/>
-      <c r="G10" s="81"/>
-      <c r="H10" s="81"/>
-      <c r="I10" s="81"/>
-      <c r="J10" s="81"/>
-      <c r="K10" s="53"/>
-      <c r="M10" s="67"/>
-      <c r="N10" s="68"/>
-      <c r="O10" s="68"/>
-      <c r="P10" s="68"/>
-      <c r="Q10" s="68"/>
-      <c r="R10" s="68"/>
-      <c r="S10" s="68"/>
-      <c r="T10" s="68"/>
-      <c r="U10" s="68"/>
-      <c r="V10" s="68"/>
-      <c r="W10" s="68"/>
-      <c r="X10" s="68"/>
-      <c r="Y10" s="68"/>
-      <c r="Z10" s="68"/>
-      <c r="AA10" s="68"/>
-      <c r="AB10" s="68"/>
-      <c r="AC10" s="68"/>
-      <c r="AD10" s="69"/>
+      <c r="E10" s="58"/>
+      <c r="F10" s="58"/>
+      <c r="G10" s="58"/>
+      <c r="H10" s="58"/>
+      <c r="I10" s="58"/>
+      <c r="J10" s="58"/>
+      <c r="K10" s="48"/>
+      <c r="M10" s="94"/>
+      <c r="N10" s="95"/>
+      <c r="O10" s="95"/>
+      <c r="P10" s="95"/>
+      <c r="Q10" s="95"/>
+      <c r="R10" s="95"/>
+      <c r="S10" s="95"/>
+      <c r="T10" s="95"/>
+      <c r="U10" s="95"/>
+      <c r="V10" s="95"/>
+      <c r="W10" s="95"/>
+      <c r="X10" s="95"/>
+      <c r="Y10" s="95"/>
+      <c r="Z10" s="95"/>
+      <c r="AA10" s="95"/>
+      <c r="AB10" s="95"/>
+      <c r="AC10" s="95"/>
+      <c r="AD10" s="96"/>
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="52" t="s">
+      <c r="A11" s="47" t="s">
         <v>44</v>
       </c>
-      <c r="B11" s="81"/>
-      <c r="C11" s="53"/>
-      <c r="D11" s="52"/>
-      <c r="E11" s="81"/>
-      <c r="F11" s="81"/>
-      <c r="G11" s="81"/>
-      <c r="H11" s="81"/>
-      <c r="I11" s="81"/>
-      <c r="J11" s="81"/>
-      <c r="K11" s="53"/>
-      <c r="M11" s="67"/>
-      <c r="N11" s="68"/>
-      <c r="O11" s="68"/>
-      <c r="P11" s="68"/>
-      <c r="Q11" s="68"/>
-      <c r="R11" s="68"/>
-      <c r="S11" s="68"/>
-      <c r="T11" s="68"/>
-      <c r="U11" s="68"/>
-      <c r="V11" s="68"/>
-      <c r="W11" s="68"/>
-      <c r="X11" s="68"/>
-      <c r="Y11" s="68"/>
-      <c r="Z11" s="68"/>
-      <c r="AA11" s="68"/>
-      <c r="AB11" s="68"/>
-      <c r="AC11" s="68"/>
-      <c r="AD11" s="69"/>
+      <c r="B11" s="58"/>
+      <c r="C11" s="48"/>
+      <c r="D11" s="47"/>
+      <c r="E11" s="58"/>
+      <c r="F11" s="58"/>
+      <c r="G11" s="58"/>
+      <c r="H11" s="58"/>
+      <c r="I11" s="58"/>
+      <c r="J11" s="58"/>
+      <c r="K11" s="48"/>
+      <c r="M11" s="94"/>
+      <c r="N11" s="95"/>
+      <c r="O11" s="95"/>
+      <c r="P11" s="95"/>
+      <c r="Q11" s="95"/>
+      <c r="R11" s="95"/>
+      <c r="S11" s="95"/>
+      <c r="T11" s="95"/>
+      <c r="U11" s="95"/>
+      <c r="V11" s="95"/>
+      <c r="W11" s="95"/>
+      <c r="X11" s="95"/>
+      <c r="Y11" s="95"/>
+      <c r="Z11" s="95"/>
+      <c r="AA11" s="95"/>
+      <c r="AB11" s="95"/>
+      <c r="AC11" s="95"/>
+      <c r="AD11" s="96"/>
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.55000000000000004">
-      <c r="M12" s="67"/>
-      <c r="N12" s="68"/>
-      <c r="O12" s="68"/>
-      <c r="P12" s="68"/>
-      <c r="Q12" s="68"/>
-      <c r="R12" s="68"/>
-      <c r="S12" s="68"/>
-      <c r="T12" s="68"/>
-      <c r="U12" s="68"/>
-      <c r="V12" s="68"/>
-      <c r="W12" s="68"/>
-      <c r="X12" s="68"/>
-      <c r="Y12" s="68"/>
-      <c r="Z12" s="68"/>
-      <c r="AA12" s="68"/>
-      <c r="AB12" s="68"/>
-      <c r="AC12" s="68"/>
-      <c r="AD12" s="69"/>
+      <c r="M12" s="94"/>
+      <c r="N12" s="95"/>
+      <c r="O12" s="95"/>
+      <c r="P12" s="95"/>
+      <c r="Q12" s="95"/>
+      <c r="R12" s="95"/>
+      <c r="S12" s="95"/>
+      <c r="T12" s="95"/>
+      <c r="U12" s="95"/>
+      <c r="V12" s="95"/>
+      <c r="W12" s="95"/>
+      <c r="X12" s="95"/>
+      <c r="Y12" s="95"/>
+      <c r="Z12" s="95"/>
+      <c r="AA12" s="95"/>
+      <c r="AB12" s="95"/>
+      <c r="AC12" s="95"/>
+      <c r="AD12" s="96"/>
     </row>
     <row r="13" spans="1:30" ht="24" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="82" t="s">
+      <c r="A13" s="60" t="s">
         <v>45</v>
       </c>
-      <c r="B13" s="83"/>
-      <c r="C13" s="83"/>
-      <c r="D13" s="83"/>
-      <c r="E13" s="83"/>
-      <c r="F13" s="83"/>
-      <c r="G13" s="83"/>
-      <c r="H13" s="83"/>
-      <c r="I13" s="83"/>
-      <c r="J13" s="83"/>
-      <c r="K13" s="84"/>
-      <c r="M13" s="67"/>
-      <c r="N13" s="68"/>
-      <c r="O13" s="68"/>
-      <c r="P13" s="68"/>
-      <c r="Q13" s="68"/>
-      <c r="R13" s="68"/>
-      <c r="S13" s="68"/>
-      <c r="T13" s="68"/>
-      <c r="U13" s="68"/>
-      <c r="V13" s="68"/>
-      <c r="W13" s="68"/>
-      <c r="X13" s="68"/>
-      <c r="Y13" s="68"/>
-      <c r="Z13" s="68"/>
-      <c r="AA13" s="68"/>
-      <c r="AB13" s="68"/>
-      <c r="AC13" s="68"/>
-      <c r="AD13" s="69"/>
+      <c r="B13" s="61"/>
+      <c r="C13" s="61"/>
+      <c r="D13" s="61"/>
+      <c r="E13" s="61"/>
+      <c r="F13" s="61"/>
+      <c r="G13" s="61"/>
+      <c r="H13" s="61"/>
+      <c r="I13" s="61"/>
+      <c r="J13" s="61"/>
+      <c r="K13" s="62"/>
+      <c r="M13" s="94"/>
+      <c r="N13" s="95"/>
+      <c r="O13" s="95"/>
+      <c r="P13" s="95"/>
+      <c r="Q13" s="95"/>
+      <c r="R13" s="95"/>
+      <c r="S13" s="95"/>
+      <c r="T13" s="95"/>
+      <c r="U13" s="95"/>
+      <c r="V13" s="95"/>
+      <c r="W13" s="95"/>
+      <c r="X13" s="95"/>
+      <c r="Y13" s="95"/>
+      <c r="Z13" s="95"/>
+      <c r="AA13" s="95"/>
+      <c r="AB13" s="95"/>
+      <c r="AC13" s="95"/>
+      <c r="AD13" s="96"/>
     </row>
     <row r="14" spans="1:30" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="93" t="s">
+      <c r="A14" s="69" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="93"/>
-      <c r="C14" s="93"/>
-      <c r="D14" s="93"/>
-      <c r="E14" s="93"/>
-      <c r="F14" s="49"/>
-      <c r="G14" s="50"/>
-      <c r="H14" s="50"/>
-      <c r="I14" s="50"/>
-      <c r="J14" s="51"/>
+      <c r="B14" s="69"/>
+      <c r="C14" s="69"/>
+      <c r="D14" s="69"/>
+      <c r="E14" s="69"/>
+      <c r="F14" s="44"/>
+      <c r="G14" s="45"/>
+      <c r="H14" s="45"/>
+      <c r="I14" s="45"/>
+      <c r="J14" s="46"/>
       <c r="K14" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="M14" s="67"/>
-      <c r="N14" s="68"/>
-      <c r="O14" s="68"/>
-      <c r="P14" s="68"/>
-      <c r="Q14" s="68"/>
-      <c r="R14" s="68"/>
-      <c r="S14" s="68"/>
-      <c r="T14" s="68"/>
-      <c r="U14" s="68"/>
-      <c r="V14" s="68"/>
-      <c r="W14" s="68"/>
-      <c r="X14" s="68"/>
-      <c r="Y14" s="68"/>
-      <c r="Z14" s="68"/>
-      <c r="AA14" s="68"/>
-      <c r="AB14" s="68"/>
-      <c r="AC14" s="68"/>
-      <c r="AD14" s="69"/>
+      <c r="M14" s="94"/>
+      <c r="N14" s="95"/>
+      <c r="O14" s="95"/>
+      <c r="P14" s="95"/>
+      <c r="Q14" s="95"/>
+      <c r="R14" s="95"/>
+      <c r="S14" s="95"/>
+      <c r="T14" s="95"/>
+      <c r="U14" s="95"/>
+      <c r="V14" s="95"/>
+      <c r="W14" s="95"/>
+      <c r="X14" s="95"/>
+      <c r="Y14" s="95"/>
+      <c r="Z14" s="95"/>
+      <c r="AA14" s="95"/>
+      <c r="AB14" s="95"/>
+      <c r="AC14" s="95"/>
+      <c r="AD14" s="96"/>
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="50"/>
-      <c r="B15" s="50"/>
-      <c r="C15" s="50"/>
-      <c r="D15" s="50"/>
-      <c r="E15" s="51"/>
-      <c r="F15" s="77" t="s">
+      <c r="A15" s="45"/>
+      <c r="B15" s="45"/>
+      <c r="C15" s="45"/>
+      <c r="D15" s="45"/>
+      <c r="E15" s="46"/>
+      <c r="F15" s="73" t="s">
         <v>3</v>
       </c>
-      <c r="G15" s="78"/>
-      <c r="H15" s="78"/>
-      <c r="I15" s="78"/>
-      <c r="J15" s="78"/>
+      <c r="G15" s="74"/>
+      <c r="H15" s="74"/>
+      <c r="I15" s="74"/>
+      <c r="J15" s="74"/>
       <c r="K15" s="21"/>
-      <c r="M15" s="67"/>
-      <c r="N15" s="68"/>
-      <c r="O15" s="68"/>
-      <c r="P15" s="68"/>
-      <c r="Q15" s="68"/>
-      <c r="R15" s="68"/>
-      <c r="S15" s="68"/>
-      <c r="T15" s="68"/>
-      <c r="U15" s="68"/>
-      <c r="V15" s="68"/>
-      <c r="W15" s="68"/>
-      <c r="X15" s="68"/>
-      <c r="Y15" s="68"/>
-      <c r="Z15" s="68"/>
-      <c r="AA15" s="68"/>
-      <c r="AB15" s="68"/>
-      <c r="AC15" s="68"/>
-      <c r="AD15" s="69"/>
+      <c r="M15" s="94"/>
+      <c r="N15" s="95"/>
+      <c r="O15" s="95"/>
+      <c r="P15" s="95"/>
+      <c r="Q15" s="95"/>
+      <c r="R15" s="95"/>
+      <c r="S15" s="95"/>
+      <c r="T15" s="95"/>
+      <c r="U15" s="95"/>
+      <c r="V15" s="95"/>
+      <c r="W15" s="95"/>
+      <c r="X15" s="95"/>
+      <c r="Y15" s="95"/>
+      <c r="Z15" s="95"/>
+      <c r="AA15" s="95"/>
+      <c r="AB15" s="95"/>
+      <c r="AC15" s="95"/>
+      <c r="AD15" s="96"/>
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="73" t="s">
+      <c r="A16" s="70" t="s">
         <v>48</v>
       </c>
-      <c r="B16" s="74"/>
-      <c r="C16" s="74"/>
-      <c r="D16" s="74"/>
-      <c r="E16" s="75"/>
-      <c r="F16" s="49">
+      <c r="B16" s="71"/>
+      <c r="C16" s="71"/>
+      <c r="D16" s="71"/>
+      <c r="E16" s="72"/>
+      <c r="F16" s="44">
         <v>0</v>
       </c>
-      <c r="G16" s="50"/>
-      <c r="H16" s="50"/>
-      <c r="I16" s="50"/>
-      <c r="J16" s="51"/>
+      <c r="G16" s="45"/>
+      <c r="H16" s="45"/>
+      <c r="I16" s="45"/>
+      <c r="J16" s="46"/>
       <c r="K16" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="M16" s="70"/>
-      <c r="N16" s="71"/>
-      <c r="O16" s="71"/>
-      <c r="P16" s="71"/>
-      <c r="Q16" s="71"/>
-      <c r="R16" s="71"/>
-      <c r="S16" s="71"/>
-      <c r="T16" s="71"/>
-      <c r="U16" s="71"/>
-      <c r="V16" s="71"/>
-      <c r="W16" s="71"/>
-      <c r="X16" s="71"/>
-      <c r="Y16" s="71"/>
-      <c r="Z16" s="71"/>
-      <c r="AA16" s="71"/>
-      <c r="AB16" s="71"/>
-      <c r="AC16" s="71"/>
-      <c r="AD16" s="72"/>
+      <c r="M16" s="97"/>
+      <c r="N16" s="57"/>
+      <c r="O16" s="57"/>
+      <c r="P16" s="57"/>
+      <c r="Q16" s="57"/>
+      <c r="R16" s="57"/>
+      <c r="S16" s="57"/>
+      <c r="T16" s="57"/>
+      <c r="U16" s="57"/>
+      <c r="V16" s="57"/>
+      <c r="W16" s="57"/>
+      <c r="X16" s="57"/>
+      <c r="Y16" s="57"/>
+      <c r="Z16" s="57"/>
+      <c r="AA16" s="57"/>
+      <c r="AB16" s="57"/>
+      <c r="AC16" s="57"/>
+      <c r="AD16" s="98"/>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="73" t="s">
+      <c r="A17" s="70" t="s">
         <v>49</v>
       </c>
-      <c r="B17" s="74"/>
-      <c r="C17" s="74"/>
-      <c r="D17" s="74"/>
-      <c r="E17" s="75"/>
-      <c r="F17" s="49">
+      <c r="B17" s="71"/>
+      <c r="C17" s="71"/>
+      <c r="D17" s="71"/>
+      <c r="E17" s="72"/>
+      <c r="F17" s="44">
         <v>0</v>
       </c>
-      <c r="G17" s="50"/>
-      <c r="H17" s="50"/>
-      <c r="I17" s="50"/>
-      <c r="J17" s="51"/>
+      <c r="G17" s="45"/>
+      <c r="H17" s="45"/>
+      <c r="I17" s="45"/>
+      <c r="J17" s="46"/>
       <c r="K17" s="6" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="73" t="s">
+      <c r="A18" s="70" t="s">
         <v>50</v>
       </c>
-      <c r="B18" s="74"/>
-      <c r="C18" s="74"/>
-      <c r="D18" s="74"/>
-      <c r="E18" s="75"/>
-      <c r="F18" s="49">
+      <c r="B18" s="71"/>
+      <c r="C18" s="71"/>
+      <c r="D18" s="71"/>
+      <c r="E18" s="72"/>
+      <c r="F18" s="44">
         <v>0</v>
       </c>
-      <c r="G18" s="50"/>
-      <c r="H18" s="50"/>
-      <c r="I18" s="50"/>
-      <c r="J18" s="51"/>
+      <c r="G18" s="45"/>
+      <c r="H18" s="45"/>
+      <c r="I18" s="45"/>
+      <c r="J18" s="46"/>
       <c r="K18" s="6" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="73" t="s">
+      <c r="A19" s="70" t="s">
         <v>51</v>
       </c>
-      <c r="B19" s="74"/>
-      <c r="C19" s="74"/>
-      <c r="D19" s="74"/>
-      <c r="E19" s="75"/>
-      <c r="F19" s="49">
+      <c r="B19" s="71"/>
+      <c r="C19" s="71"/>
+      <c r="D19" s="71"/>
+      <c r="E19" s="72"/>
+      <c r="F19" s="44">
         <v>0</v>
       </c>
-      <c r="G19" s="50"/>
-      <c r="H19" s="50"/>
-      <c r="I19" s="50"/>
-      <c r="J19" s="51"/>
+      <c r="G19" s="45"/>
+      <c r="H19" s="45"/>
+      <c r="I19" s="45"/>
+      <c r="J19" s="46"/>
       <c r="K19" s="6" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="92" t="s">
+      <c r="A20" s="75" t="s">
         <v>52</v>
       </c>
-      <c r="B20" s="92"/>
-      <c r="C20" s="92"/>
-      <c r="D20" s="92"/>
-      <c r="E20" s="92"/>
-      <c r="F20" s="63">
+      <c r="B20" s="75"/>
+      <c r="C20" s="75"/>
+      <c r="D20" s="75"/>
+      <c r="E20" s="75"/>
+      <c r="F20" s="76">
         <f>SUM(F16:J19)</f>
         <v>0</v>
       </c>
-      <c r="G20" s="63"/>
-      <c r="H20" s="63"/>
-      <c r="I20" s="63"/>
-      <c r="J20" s="63"/>
+      <c r="G20" s="76"/>
+      <c r="H20" s="76"/>
+      <c r="I20" s="76"/>
+      <c r="J20" s="76"/>
       <c r="K20" s="11" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" s="82" t="s">
+      <c r="A22" s="60" t="s">
         <v>53</v>
       </c>
-      <c r="B22" s="83"/>
-      <c r="C22" s="83"/>
-      <c r="D22" s="83"/>
-      <c r="E22" s="83"/>
-      <c r="F22" s="83"/>
-      <c r="G22" s="83"/>
-      <c r="H22" s="83"/>
-      <c r="I22" s="83"/>
-      <c r="J22" s="83"/>
-      <c r="K22" s="84"/>
+      <c r="B22" s="61"/>
+      <c r="C22" s="61"/>
+      <c r="D22" s="61"/>
+      <c r="E22" s="61"/>
+      <c r="F22" s="61"/>
+      <c r="G22" s="61"/>
+      <c r="H22" s="61"/>
+      <c r="I22" s="61"/>
+      <c r="J22" s="61"/>
+      <c r="K22" s="62"/>
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="91" t="s">
+      <c r="A23" s="77" t="s">
         <v>54</v>
       </c>
-      <c r="B23" s="91"/>
-      <c r="C23" s="91"/>
-      <c r="D23" s="91"/>
-      <c r="E23" s="91"/>
-      <c r="F23" s="49"/>
-      <c r="G23" s="50"/>
-      <c r="H23" s="50"/>
-      <c r="I23" s="50"/>
-      <c r="J23" s="50"/>
-      <c r="K23" s="51"/>
-      <c r="M23" s="85" t="s">
+      <c r="B23" s="77"/>
+      <c r="C23" s="77"/>
+      <c r="D23" s="77"/>
+      <c r="E23" s="77"/>
+      <c r="F23" s="44"/>
+      <c r="G23" s="45"/>
+      <c r="H23" s="45"/>
+      <c r="I23" s="45"/>
+      <c r="J23" s="45"/>
+      <c r="K23" s="46"/>
+      <c r="M23" s="81" t="s">
         <v>62</v>
       </c>
-      <c r="N23" s="86"/>
-      <c r="O23" s="86"/>
-      <c r="P23" s="86"/>
-      <c r="Q23" s="86"/>
-      <c r="R23" s="86"/>
-      <c r="S23" s="86"/>
-      <c r="T23" s="86"/>
-      <c r="U23" s="86"/>
-      <c r="V23" s="86"/>
-      <c r="W23" s="87"/>
+      <c r="N23" s="82"/>
+      <c r="O23" s="82"/>
+      <c r="P23" s="82"/>
+      <c r="Q23" s="82"/>
+      <c r="R23" s="82"/>
+      <c r="S23" s="82"/>
+      <c r="T23" s="82"/>
+      <c r="U23" s="82"/>
+      <c r="V23" s="82"/>
+      <c r="W23" s="83"/>
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" s="49"/>
-      <c r="B24" s="50"/>
-      <c r="C24" s="50"/>
-      <c r="D24" s="50"/>
-      <c r="E24" s="51"/>
-      <c r="F24" s="63" t="s">
+      <c r="A24" s="44"/>
+      <c r="B24" s="45"/>
+      <c r="C24" s="45"/>
+      <c r="D24" s="45"/>
+      <c r="E24" s="46"/>
+      <c r="F24" s="76" t="s">
         <v>55</v>
       </c>
-      <c r="G24" s="63"/>
-      <c r="H24" s="63"/>
-      <c r="I24" s="63"/>
-      <c r="J24" s="63"/>
-      <c r="K24" s="63"/>
-      <c r="M24" s="77" t="s">
+      <c r="G24" s="76"/>
+      <c r="H24" s="76"/>
+      <c r="I24" s="76"/>
+      <c r="J24" s="76"/>
+      <c r="K24" s="76"/>
+      <c r="M24" s="73" t="s">
         <v>60</v>
       </c>
-      <c r="N24" s="79"/>
-      <c r="O24" s="63" t="s">
+      <c r="N24" s="84"/>
+      <c r="O24" s="76" t="s">
         <v>61</v>
       </c>
-      <c r="P24" s="63"/>
-      <c r="Q24" s="63" t="s">
+      <c r="P24" s="76"/>
+      <c r="Q24" s="76" t="s">
         <v>10</v>
       </c>
-      <c r="R24" s="63"/>
-      <c r="S24" s="63"/>
-      <c r="T24" s="63"/>
-      <c r="U24" s="63"/>
-      <c r="V24" s="63"/>
-      <c r="W24" s="63"/>
+      <c r="R24" s="76"/>
+      <c r="S24" s="76"/>
+      <c r="T24" s="76"/>
+      <c r="U24" s="76"/>
+      <c r="V24" s="76"/>
+      <c r="W24" s="76"/>
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25" s="88" t="s">
+      <c r="A25" s="78" t="s">
         <v>56</v>
       </c>
-      <c r="B25" s="89"/>
-      <c r="C25" s="89"/>
-      <c r="D25" s="89"/>
-      <c r="E25" s="90"/>
-      <c r="F25" s="49">
+      <c r="B25" s="79"/>
+      <c r="C25" s="79"/>
+      <c r="D25" s="79"/>
+      <c r="E25" s="80"/>
+      <c r="F25" s="44">
         <v>0</v>
       </c>
-      <c r="G25" s="50"/>
-      <c r="H25" s="50"/>
-      <c r="I25" s="50"/>
-      <c r="J25" s="50"/>
-      <c r="K25" s="51"/>
-      <c r="M25" s="49">
+      <c r="G25" s="45"/>
+      <c r="H25" s="45"/>
+      <c r="I25" s="45"/>
+      <c r="J25" s="45"/>
+      <c r="K25" s="46"/>
+      <c r="M25" s="44">
         <v>1</v>
       </c>
-      <c r="N25" s="51"/>
-      <c r="O25" s="49" t="s">
+      <c r="N25" s="46"/>
+      <c r="O25" s="44" t="s">
         <v>63</v>
       </c>
-      <c r="P25" s="51"/>
-      <c r="Q25" s="52" t="s">
+      <c r="P25" s="46"/>
+      <c r="Q25" s="47" t="s">
         <v>67</v>
       </c>
-      <c r="R25" s="81"/>
-      <c r="S25" s="81"/>
-      <c r="T25" s="81"/>
-      <c r="U25" s="81"/>
-      <c r="V25" s="81"/>
-      <c r="W25" s="53"/>
+      <c r="R25" s="58"/>
+      <c r="S25" s="58"/>
+      <c r="T25" s="58"/>
+      <c r="U25" s="58"/>
+      <c r="V25" s="58"/>
+      <c r="W25" s="48"/>
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" s="88" t="s">
+      <c r="A26" s="78" t="s">
         <v>57</v>
       </c>
-      <c r="B26" s="89"/>
-      <c r="C26" s="89"/>
-      <c r="D26" s="89"/>
-      <c r="E26" s="90"/>
-      <c r="F26" s="49">
+      <c r="B26" s="79"/>
+      <c r="C26" s="79"/>
+      <c r="D26" s="79"/>
+      <c r="E26" s="80"/>
+      <c r="F26" s="44">
         <v>0</v>
       </c>
-      <c r="G26" s="50"/>
-      <c r="H26" s="50"/>
-      <c r="I26" s="50"/>
-      <c r="J26" s="50"/>
-      <c r="K26" s="51"/>
-      <c r="M26" s="49">
+      <c r="G26" s="45"/>
+      <c r="H26" s="45"/>
+      <c r="I26" s="45"/>
+      <c r="J26" s="45"/>
+      <c r="K26" s="46"/>
+      <c r="M26" s="44">
         <v>2</v>
       </c>
-      <c r="N26" s="51"/>
-      <c r="O26" s="49" t="s">
+      <c r="N26" s="46"/>
+      <c r="O26" s="44" t="s">
         <v>64</v>
       </c>
-      <c r="P26" s="51"/>
-      <c r="Q26" s="52" t="s">
+      <c r="P26" s="46"/>
+      <c r="Q26" s="47" t="s">
         <v>66</v>
       </c>
-      <c r="R26" s="81"/>
-      <c r="S26" s="81"/>
-      <c r="T26" s="81"/>
-      <c r="U26" s="81"/>
-      <c r="V26" s="81"/>
-      <c r="W26" s="53"/>
+      <c r="R26" s="58"/>
+      <c r="S26" s="58"/>
+      <c r="T26" s="58"/>
+      <c r="U26" s="58"/>
+      <c r="V26" s="58"/>
+      <c r="W26" s="48"/>
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" s="88" t="s">
+      <c r="A27" s="78" t="s">
         <v>58</v>
       </c>
-      <c r="B27" s="89"/>
-      <c r="C27" s="89"/>
-      <c r="D27" s="89"/>
-      <c r="E27" s="90"/>
-      <c r="F27" s="49">
+      <c r="B27" s="79"/>
+      <c r="C27" s="79"/>
+      <c r="D27" s="79"/>
+      <c r="E27" s="80"/>
+      <c r="F27" s="44">
         <v>0</v>
       </c>
-      <c r="G27" s="50"/>
-      <c r="H27" s="50"/>
-      <c r="I27" s="50"/>
-      <c r="J27" s="50"/>
-      <c r="K27" s="51"/>
-      <c r="M27" s="49">
+      <c r="G27" s="45"/>
+      <c r="H27" s="45"/>
+      <c r="I27" s="45"/>
+      <c r="J27" s="45"/>
+      <c r="K27" s="46"/>
+      <c r="M27" s="44">
         <v>3</v>
       </c>
-      <c r="N27" s="51"/>
-      <c r="O27" s="49" t="s">
+      <c r="N27" s="46"/>
+      <c r="O27" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="P27" s="51"/>
-      <c r="Q27" s="52" t="s">
+      <c r="P27" s="46"/>
+      <c r="Q27" s="47" t="s">
         <v>68</v>
       </c>
-      <c r="R27" s="81"/>
-      <c r="S27" s="81"/>
-      <c r="T27" s="81"/>
-      <c r="U27" s="81"/>
-      <c r="V27" s="81"/>
-      <c r="W27" s="53"/>
+      <c r="R27" s="58"/>
+      <c r="S27" s="58"/>
+      <c r="T27" s="58"/>
+      <c r="U27" s="58"/>
+      <c r="V27" s="58"/>
+      <c r="W27" s="48"/>
     </row>
     <row r="28" spans="1:23" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28" s="88" t="s">
+      <c r="A28" s="78" t="s">
         <v>59</v>
       </c>
-      <c r="B28" s="89"/>
-      <c r="C28" s="89"/>
-      <c r="D28" s="89"/>
-      <c r="E28" s="90"/>
-      <c r="F28" s="49">
+      <c r="B28" s="79"/>
+      <c r="C28" s="79"/>
+      <c r="D28" s="79"/>
+      <c r="E28" s="80"/>
+      <c r="F28" s="44">
         <v>0</v>
       </c>
-      <c r="G28" s="50"/>
-      <c r="H28" s="50"/>
-      <c r="I28" s="50"/>
-      <c r="J28" s="50"/>
-      <c r="K28" s="51"/>
-      <c r="M28" s="49">
+      <c r="G28" s="45"/>
+      <c r="H28" s="45"/>
+      <c r="I28" s="45"/>
+      <c r="J28" s="45"/>
+      <c r="K28" s="46"/>
+      <c r="M28" s="44">
         <v>4</v>
       </c>
-      <c r="N28" s="51"/>
-      <c r="O28" s="49" t="s">
+      <c r="N28" s="46"/>
+      <c r="O28" s="44" t="s">
         <v>65</v>
       </c>
-      <c r="P28" s="51"/>
-      <c r="Q28" s="52" t="s">
+      <c r="P28" s="46"/>
+      <c r="Q28" s="47" t="s">
         <v>85</v>
       </c>
-      <c r="R28" s="81"/>
-      <c r="S28" s="81"/>
-      <c r="T28" s="81"/>
-      <c r="U28" s="81"/>
-      <c r="V28" s="81"/>
-      <c r="W28" s="53"/>
+      <c r="R28" s="58"/>
+      <c r="S28" s="58"/>
+      <c r="T28" s="58"/>
+      <c r="U28" s="58"/>
+      <c r="V28" s="58"/>
+      <c r="W28" s="48"/>
     </row>
     <row r="29" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="B29" s="49"/>
-      <c r="C29" s="50"/>
-      <c r="D29" s="50"/>
-      <c r="E29" s="50"/>
-      <c r="F29" s="50"/>
-      <c r="G29" s="50"/>
-      <c r="H29" s="50"/>
-      <c r="I29" s="50"/>
-      <c r="J29" s="50"/>
-      <c r="K29" s="51"/>
+      <c r="B29" s="44"/>
+      <c r="C29" s="45"/>
+      <c r="D29" s="45"/>
+      <c r="E29" s="45"/>
+      <c r="F29" s="45"/>
+      <c r="G29" s="45"/>
+      <c r="H29" s="45"/>
+      <c r="I29" s="45"/>
+      <c r="J29" s="45"/>
+      <c r="K29" s="46"/>
       <c r="M29" s="14"/>
       <c r="N29" s="14"/>
       <c r="O29" s="14"/>
@@ -6967,196 +8576,124 @@
       <c r="W29" s="19"/>
     </row>
     <row r="31" spans="1:23" x14ac:dyDescent="0.55000000000000004">
-      <c r="A31" s="82" t="s">
+      <c r="A31" s="60" t="s">
         <v>69</v>
       </c>
-      <c r="B31" s="83"/>
-      <c r="C31" s="83"/>
-      <c r="D31" s="83"/>
-      <c r="E31" s="83"/>
-      <c r="F31" s="83"/>
-      <c r="G31" s="83"/>
-      <c r="H31" s="83"/>
-      <c r="I31" s="83"/>
-      <c r="J31" s="83"/>
-      <c r="K31" s="84"/>
+      <c r="B31" s="61"/>
+      <c r="C31" s="61"/>
+      <c r="D31" s="61"/>
+      <c r="E31" s="61"/>
+      <c r="F31" s="61"/>
+      <c r="G31" s="61"/>
+      <c r="H31" s="61"/>
+      <c r="I31" s="61"/>
+      <c r="J31" s="61"/>
+      <c r="K31" s="62"/>
     </row>
     <row r="32" spans="1:23" x14ac:dyDescent="0.55000000000000004">
-      <c r="A32" s="73" t="s">
+      <c r="A32" s="70" t="s">
         <v>73</v>
       </c>
-      <c r="B32" s="74"/>
-      <c r="C32" s="75"/>
-      <c r="D32" s="54"/>
-      <c r="E32" s="55"/>
-      <c r="F32" s="55"/>
-      <c r="G32" s="55"/>
-      <c r="H32" s="55"/>
-      <c r="I32" s="56"/>
-      <c r="J32" s="76" t="s">
+      <c r="B32" s="71"/>
+      <c r="C32" s="72"/>
+      <c r="D32" s="49"/>
+      <c r="E32" s="50"/>
+      <c r="F32" s="50"/>
+      <c r="G32" s="50"/>
+      <c r="H32" s="50"/>
+      <c r="I32" s="51"/>
+      <c r="J32" s="59" t="s">
         <v>72</v>
       </c>
-      <c r="K32" s="76"/>
+      <c r="K32" s="59"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A33" s="73" t="s">
+      <c r="A33" s="70" t="s">
         <v>74</v>
       </c>
-      <c r="B33" s="74"/>
-      <c r="C33" s="75"/>
-      <c r="D33" s="54"/>
-      <c r="E33" s="55"/>
-      <c r="F33" s="55"/>
-      <c r="G33" s="55"/>
-      <c r="H33" s="55"/>
-      <c r="I33" s="56"/>
-      <c r="J33" s="76" t="s">
+      <c r="B33" s="71"/>
+      <c r="C33" s="72"/>
+      <c r="D33" s="49"/>
+      <c r="E33" s="50"/>
+      <c r="F33" s="50"/>
+      <c r="G33" s="50"/>
+      <c r="H33" s="50"/>
+      <c r="I33" s="51"/>
+      <c r="J33" s="59" t="s">
         <v>72</v>
       </c>
-      <c r="K33" s="76"/>
+      <c r="K33" s="59"/>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A34" s="73" t="s">
+      <c r="A34" s="70" t="s">
         <v>75</v>
       </c>
-      <c r="B34" s="74"/>
-      <c r="C34" s="75"/>
-      <c r="D34" s="54"/>
-      <c r="E34" s="55"/>
-      <c r="F34" s="55"/>
-      <c r="G34" s="55"/>
-      <c r="H34" s="55"/>
-      <c r="I34" s="56"/>
-      <c r="J34" s="76" t="s">
+      <c r="B34" s="71"/>
+      <c r="C34" s="72"/>
+      <c r="D34" s="49"/>
+      <c r="E34" s="50"/>
+      <c r="F34" s="50"/>
+      <c r="G34" s="50"/>
+      <c r="H34" s="50"/>
+      <c r="I34" s="51"/>
+      <c r="J34" s="59" t="s">
         <v>72</v>
       </c>
-      <c r="K34" s="76"/>
+      <c r="K34" s="59"/>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A35" s="73" t="s">
+      <c r="A35" s="70" t="s">
         <v>76</v>
       </c>
-      <c r="B35" s="74"/>
-      <c r="C35" s="75"/>
-      <c r="D35" s="54"/>
-      <c r="E35" s="55"/>
-      <c r="F35" s="55"/>
-      <c r="G35" s="55"/>
-      <c r="H35" s="55"/>
-      <c r="I35" s="56"/>
-      <c r="J35" s="76" t="s">
+      <c r="B35" s="71"/>
+      <c r="C35" s="72"/>
+      <c r="D35" s="49"/>
+      <c r="E35" s="50"/>
+      <c r="F35" s="50"/>
+      <c r="G35" s="50"/>
+      <c r="H35" s="50"/>
+      <c r="I35" s="51"/>
+      <c r="J35" s="59" t="s">
         <v>72</v>
       </c>
-      <c r="K35" s="76"/>
+      <c r="K35" s="59"/>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A36" s="57" t="s">
+      <c r="A36" s="85" t="s">
         <v>71</v>
       </c>
-      <c r="B36" s="58"/>
-      <c r="C36" s="59"/>
-      <c r="D36" s="77"/>
-      <c r="E36" s="78"/>
-      <c r="F36" s="78"/>
-      <c r="G36" s="78"/>
-      <c r="H36" s="78"/>
-      <c r="I36" s="79"/>
-      <c r="J36" s="80" t="s">
+      <c r="B36" s="86"/>
+      <c r="C36" s="87"/>
+      <c r="D36" s="73"/>
+      <c r="E36" s="74"/>
+      <c r="F36" s="74"/>
+      <c r="G36" s="74"/>
+      <c r="H36" s="74"/>
+      <c r="I36" s="84"/>
+      <c r="J36" s="99" t="s">
         <v>72</v>
       </c>
-      <c r="K36" s="80"/>
+      <c r="K36" s="99"/>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A37" s="57" t="s">
+      <c r="A37" s="85" t="s">
         <v>77</v>
       </c>
-      <c r="B37" s="58"/>
-      <c r="C37" s="59"/>
-      <c r="D37" s="60"/>
-      <c r="E37" s="62"/>
-      <c r="F37" s="62"/>
-      <c r="G37" s="62"/>
-      <c r="H37" s="62"/>
-      <c r="I37" s="61"/>
-      <c r="J37" s="60" t="s">
+      <c r="B37" s="86"/>
+      <c r="C37" s="87"/>
+      <c r="D37" s="88"/>
+      <c r="E37" s="90"/>
+      <c r="F37" s="90"/>
+      <c r="G37" s="90"/>
+      <c r="H37" s="90"/>
+      <c r="I37" s="89"/>
+      <c r="J37" s="88" t="s">
         <v>78</v>
       </c>
-      <c r="K37" s="61"/>
+      <c r="K37" s="89"/>
     </row>
   </sheetData>
   <mergeCells count="88">
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="D3:H3"/>
-    <mergeCell ref="D7:K7"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="I5:K5"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="I6:K6"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="D11:K11"/>
-    <mergeCell ref="A13:K13"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="D8:K8"/>
-    <mergeCell ref="A9:C10"/>
-    <mergeCell ref="D9:K9"/>
-    <mergeCell ref="D10:K10"/>
-    <mergeCell ref="A14:E14"/>
-    <mergeCell ref="F14:J14"/>
-    <mergeCell ref="A16:E16"/>
-    <mergeCell ref="A17:E17"/>
-    <mergeCell ref="A18:E18"/>
-    <mergeCell ref="F15:J15"/>
-    <mergeCell ref="F16:J16"/>
-    <mergeCell ref="F17:J17"/>
-    <mergeCell ref="A15:E15"/>
-    <mergeCell ref="F18:J18"/>
-    <mergeCell ref="F19:J19"/>
-    <mergeCell ref="A20:E20"/>
-    <mergeCell ref="F20:J20"/>
-    <mergeCell ref="A19:E19"/>
-    <mergeCell ref="A22:K22"/>
-    <mergeCell ref="A23:E23"/>
-    <mergeCell ref="F23:K23"/>
-    <mergeCell ref="F24:K24"/>
-    <mergeCell ref="A24:E24"/>
-    <mergeCell ref="A25:E25"/>
-    <mergeCell ref="A26:E26"/>
-    <mergeCell ref="A27:E27"/>
-    <mergeCell ref="A28:E28"/>
-    <mergeCell ref="F25:K25"/>
-    <mergeCell ref="F26:K26"/>
-    <mergeCell ref="F27:K27"/>
-    <mergeCell ref="F28:K28"/>
-    <mergeCell ref="M23:W23"/>
-    <mergeCell ref="Q25:W25"/>
-    <mergeCell ref="Q26:W26"/>
-    <mergeCell ref="Q27:W27"/>
-    <mergeCell ref="O24:P24"/>
-    <mergeCell ref="O25:P25"/>
-    <mergeCell ref="O26:P26"/>
-    <mergeCell ref="O27:P27"/>
-    <mergeCell ref="M24:N24"/>
-    <mergeCell ref="M25:N25"/>
-    <mergeCell ref="M26:N26"/>
-    <mergeCell ref="M27:N27"/>
-    <mergeCell ref="D34:I34"/>
-    <mergeCell ref="J34:K34"/>
-    <mergeCell ref="Q28:W28"/>
-    <mergeCell ref="A31:K31"/>
-    <mergeCell ref="B29:K29"/>
-    <mergeCell ref="A32:C32"/>
-    <mergeCell ref="J32:K32"/>
-    <mergeCell ref="D32:I32"/>
-    <mergeCell ref="O28:P28"/>
-    <mergeCell ref="M28:N28"/>
     <mergeCell ref="A37:C37"/>
     <mergeCell ref="J37:K37"/>
     <mergeCell ref="D37:I37"/>
@@ -7173,6 +8710,78 @@
     <mergeCell ref="D33:I33"/>
     <mergeCell ref="J33:K33"/>
     <mergeCell ref="A34:C34"/>
+    <mergeCell ref="D34:I34"/>
+    <mergeCell ref="J34:K34"/>
+    <mergeCell ref="Q28:W28"/>
+    <mergeCell ref="A31:K31"/>
+    <mergeCell ref="B29:K29"/>
+    <mergeCell ref="A32:C32"/>
+    <mergeCell ref="J32:K32"/>
+    <mergeCell ref="D32:I32"/>
+    <mergeCell ref="O28:P28"/>
+    <mergeCell ref="M28:N28"/>
+    <mergeCell ref="M23:W23"/>
+    <mergeCell ref="Q25:W25"/>
+    <mergeCell ref="Q26:W26"/>
+    <mergeCell ref="Q27:W27"/>
+    <mergeCell ref="O24:P24"/>
+    <mergeCell ref="O25:P25"/>
+    <mergeCell ref="O26:P26"/>
+    <mergeCell ref="O27:P27"/>
+    <mergeCell ref="M24:N24"/>
+    <mergeCell ref="M25:N25"/>
+    <mergeCell ref="M26:N26"/>
+    <mergeCell ref="M27:N27"/>
+    <mergeCell ref="A26:E26"/>
+    <mergeCell ref="A27:E27"/>
+    <mergeCell ref="A28:E28"/>
+    <mergeCell ref="F25:K25"/>
+    <mergeCell ref="F26:K26"/>
+    <mergeCell ref="F27:K27"/>
+    <mergeCell ref="F28:K28"/>
+    <mergeCell ref="A23:E23"/>
+    <mergeCell ref="F23:K23"/>
+    <mergeCell ref="F24:K24"/>
+    <mergeCell ref="A24:E24"/>
+    <mergeCell ref="A25:E25"/>
+    <mergeCell ref="F19:J19"/>
+    <mergeCell ref="A20:E20"/>
+    <mergeCell ref="F20:J20"/>
+    <mergeCell ref="A19:E19"/>
+    <mergeCell ref="A22:K22"/>
+    <mergeCell ref="A14:E14"/>
+    <mergeCell ref="F14:J14"/>
+    <mergeCell ref="A16:E16"/>
+    <mergeCell ref="A17:E17"/>
+    <mergeCell ref="A18:E18"/>
+    <mergeCell ref="F15:J15"/>
+    <mergeCell ref="F16:J16"/>
+    <mergeCell ref="F17:J17"/>
+    <mergeCell ref="A15:E15"/>
+    <mergeCell ref="F18:J18"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="D11:K11"/>
+    <mergeCell ref="A13:K13"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="D8:K8"/>
+    <mergeCell ref="A9:C10"/>
+    <mergeCell ref="D9:K9"/>
+    <mergeCell ref="D10:K10"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="D3:H3"/>
+    <mergeCell ref="D7:K7"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="I5:K5"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="I6:K6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>